<commit_message>
New checklist, french version : comments corrected
</commit_message>
<xml_diff>
--- a/Checklists/Mobile_App_Security_Checklist-French.xlsx
+++ b/Checklists/Mobile_App_Security_Checklist-French.xlsx
@@ -5,12 +5,12 @@
   <workbookPr showInkAnnotation="0" codeName="ThisWorkbook" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projects\MASVS_MSTG\owasp-mstg\Checklists\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{170E6F3A-F74A-41BE-8B1B-A0463D46F0D8}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02569E04-4A59-4215-A33C-D36B9415AA11}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6945" tabRatio="500" firstSheet="4" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6945" tabRatio="500" firstSheet="3" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tableau de Bord" sheetId="6" r:id="rId1"/>
@@ -312,9 +312,6 @@
     <t>Nom du fichier</t>
   </si>
   <si>
-    <t>V1: Architecture, Conception et Modélisation des menaces</t>
-  </si>
-  <si>
     <t>Score de conformité du MASVS ( / 5)</t>
   </si>
   <si>
@@ -336,9 +333,6 @@
     <t>Statut</t>
   </si>
   <si>
-    <t>Architecture, conception et modélisation des menaces</t>
-  </si>
-  <si>
     <t>Cryptographie</t>
   </si>
   <si>
@@ -685,9 +679,6 @@
   </si>
   <si>
     <t>V7: Qualité du code et paramètres de génération</t>
-  </si>
-  <si>
-    <t>V6: Intéraction avec les Plateformes</t>
   </si>
   <si>
     <t>Score de Conformité au MASVS ( / 5)</t>
@@ -756,9 +747,6 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve"> Intéraction avec les Plateformes</t>
-  </si>
-  <si>
     <t xml:space="preserve">Exigences de Vérification détaillées </t>
   </si>
   <si>
@@ -804,9 +792,6 @@
     <t xml:space="preserve"> Synchronisation avec le MASVS (mise à jour du domaine 2), mise à jour des liens vers le nouveau Gitbook</t>
   </si>
   <si>
-    <t>Version en ligne de MSTG</t>
-  </si>
-  <si>
     <t>Version du MASVS</t>
   </si>
   <si>
@@ -832,6 +817,21 @@
   </si>
   <si>
     <t>Mise à jour des liens vers le guide 1.1.0</t>
+  </si>
+  <si>
+    <t>V1:Architecture, Design et Modèle de Menaces</t>
+  </si>
+  <si>
+    <t>Architecture, Design et Modèle de Menaces</t>
+  </si>
+  <si>
+    <t>Interactions avec la Plateforme</t>
+  </si>
+  <si>
+    <t>V6: Interactions avec la Plateforme</t>
+  </si>
+  <si>
+    <t>Version en ligne du MSTG</t>
   </si>
 </sst>
 </file>
@@ -1875,133 +1875,133 @@
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="36" xfId="9" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="12" borderId="21" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="12" borderId="20" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="12" borderId="22" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="1" fontId="13" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="13" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="13" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="13" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="13" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="13" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="13" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="13" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="37" xfId="9" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="13" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="13" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="13" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="13" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="13" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="13" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="13" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="13" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="21" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="20" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="22" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="62">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -2215,7 +2215,7 @@
               <c:strCache>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>V1: Architecture, Conception et Modélisation des menaces</c:v>
+                  <c:v>V1:Architecture, Design et Modèle de Menaces</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>V2: Stockage des données et Respect de la Vie Privée</c:v>
@@ -2230,7 +2230,7 @@
                   <c:v>V5: Communication Réseau</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>V6: Intéraction avec les Plateformes</c:v>
+                  <c:v>V6: Interactions avec la Plateforme</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>V7: Qualité du code et paramètres de génération</c:v>
@@ -2567,7 +2567,7 @@
               <c:strCache>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>V1: Architecture, Conception et Modélisation des menaces</c:v>
+                  <c:v>V1:Architecture, Design et Modèle de Menaces</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>V2: Stockage des données et Respect de la Vie Privée</c:v>
@@ -2582,7 +2582,7 @@
                   <c:v>V5: Communication Réseau</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>V6: Intéraction avec les Plateformes</c:v>
+                  <c:v>V6: Interactions avec la Plateforme</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>V7: Qualité du code et paramètres de génération</c:v>
@@ -3280,8 +3280,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="B1:D47"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView showGridLines="0" topLeftCell="A57" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -3293,68 +3293,68 @@
   <sheetData>
     <row r="1" spans="2:4" ht="8.1" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B2" s="102" t="s">
-        <v>233</v>
-      </c>
-      <c r="C2" s="103"/>
-      <c r="D2" s="104"/>
+      <c r="B2" s="111" t="s">
+        <v>230</v>
+      </c>
+      <c r="C2" s="112"/>
+      <c r="D2" s="113"/>
     </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B3" s="105"/>
-      <c r="C3" s="106"/>
-      <c r="D3" s="107"/>
+      <c r="B3" s="114"/>
+      <c r="C3" s="115"/>
+      <c r="D3" s="116"/>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B4" s="105"/>
-      <c r="C4" s="106"/>
-      <c r="D4" s="107"/>
+      <c r="B4" s="114"/>
+      <c r="C4" s="115"/>
+      <c r="D4" s="116"/>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B5" s="105"/>
-      <c r="C5" s="106"/>
-      <c r="D5" s="107"/>
+      <c r="B5" s="114"/>
+      <c r="C5" s="115"/>
+      <c r="D5" s="116"/>
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B6" s="105"/>
-      <c r="C6" s="106"/>
-      <c r="D6" s="107"/>
+      <c r="B6" s="114"/>
+      <c r="C6" s="115"/>
+      <c r="D6" s="116"/>
     </row>
     <row r="7" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B7" s="105"/>
-      <c r="C7" s="106"/>
-      <c r="D7" s="107"/>
+      <c r="B7" s="114"/>
+      <c r="C7" s="115"/>
+      <c r="D7" s="116"/>
     </row>
     <row r="8" spans="2:4" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="108"/>
-      <c r="C8" s="109"/>
-      <c r="D8" s="110"/>
+      <c r="B8" s="117"/>
+      <c r="C8" s="118"/>
+      <c r="D8" s="119"/>
     </row>
     <row r="9" spans="2:4" ht="18" x14ac:dyDescent="0.35">
-      <c r="B9" s="111" t="s">
+      <c r="B9" s="120" t="s">
         <v>66</v>
       </c>
-      <c r="C9" s="112"/>
-      <c r="D9" s="113"/>
+      <c r="C9" s="108"/>
+      <c r="D9" s="109"/>
     </row>
     <row r="10" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="C10" s="2"/>
       <c r="D10" s="3"/>
     </row>
     <row r="11" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B11" s="98" t="s">
-        <v>251</v>
-      </c>
-      <c r="C11" s="99"/>
+      <c r="B11" s="106" t="s">
+        <v>246</v>
+      </c>
+      <c r="C11" s="107"/>
       <c r="D11" s="12" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
     </row>
     <row r="12" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B12" s="79" t="s">
-        <v>250</v>
+        <v>259</v>
       </c>
       <c r="C12" s="80"/>
       <c r="D12" s="93" t="str">
@@ -3370,249 +3370,247 @@
       <c r="D13" s="12"/>
     </row>
     <row r="14" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B14" s="100" t="s">
+      <c r="B14" s="101" t="s">
+        <v>215</v>
+      </c>
+      <c r="C14" s="110"/>
+      <c r="D14" s="12"/>
+    </row>
+    <row r="15" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B15" s="106" t="s">
+        <v>87</v>
+      </c>
+      <c r="C15" s="107"/>
+      <c r="D15" s="12"/>
+    </row>
+    <row r="16" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B16" s="106" t="s">
+        <v>216</v>
+      </c>
+      <c r="C16" s="107"/>
+      <c r="D16" s="12"/>
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B17" s="106" t="s">
+        <v>88</v>
+      </c>
+      <c r="C17" s="107"/>
+      <c r="D17" s="12"/>
+    </row>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B18" s="106" t="s">
+        <v>217</v>
+      </c>
+      <c r="C18" s="107"/>
+      <c r="D18" s="12" t="s">
         <v>218</v>
       </c>
-      <c r="C14" s="101"/>
-      <c r="D14" s="12"/>
-    </row>
-    <row r="15" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B15" s="98" t="s">
-        <v>87</v>
-      </c>
-      <c r="C15" s="99"/>
-      <c r="D15" s="12"/>
-    </row>
-    <row r="16" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B16" s="98" t="s">
+    </row>
+    <row r="19" spans="2:4" ht="70.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B19" s="106" t="s">
         <v>219</v>
       </c>
-      <c r="C16" s="99"/>
-      <c r="D16" s="12"/>
-    </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B17" s="98" t="s">
-        <v>88</v>
-      </c>
-      <c r="C17" s="99"/>
-      <c r="D17" s="12"/>
-    </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B18" s="98" t="s">
+      <c r="C19" s="107"/>
+      <c r="D19" s="12" t="s">
         <v>220</v>
       </c>
-      <c r="C18" s="99"/>
-      <c r="D18" s="12" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="19" spans="2:4" ht="70.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="98" t="s">
-        <v>222</v>
-      </c>
-      <c r="C19" s="99"/>
-      <c r="D19" s="12" t="s">
-        <v>223</v>
-      </c>
     </row>
     <row r="20" spans="2:4" ht="18" x14ac:dyDescent="0.35">
-      <c r="B20" s="112"/>
-      <c r="C20" s="112"/>
-      <c r="D20" s="113"/>
+      <c r="B20" s="108"/>
+      <c r="C20" s="108"/>
+      <c r="D20" s="109"/>
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B21" s="1" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="C21" s="2"/>
       <c r="D21" s="3"/>
     </row>
     <row r="22" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B22" s="78" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="C22" s="4"/>
       <c r="D22" s="12"/>
     </row>
     <row r="23" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B23" s="98" t="s">
-        <v>226</v>
-      </c>
-      <c r="C23" s="99"/>
+      <c r="B23" s="106" t="s">
+        <v>223</v>
+      </c>
+      <c r="C23" s="107"/>
       <c r="D23" s="12"/>
     </row>
     <row r="24" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B24" s="98" t="s">
+      <c r="B24" s="106" t="s">
         <v>89</v>
       </c>
-      <c r="C24" s="99"/>
+      <c r="C24" s="107"/>
       <c r="D24" s="12"/>
     </row>
     <row r="25" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B25" s="98" t="s">
+      <c r="B25" s="106" t="s">
         <v>64</v>
       </c>
-      <c r="C25" s="99"/>
+      <c r="C25" s="107"/>
       <c r="D25" s="12"/>
     </row>
     <row r="26" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B26" s="98" t="s">
-        <v>227</v>
-      </c>
-      <c r="C26" s="99"/>
+      <c r="B26" s="106" t="s">
+        <v>224</v>
+      </c>
+      <c r="C26" s="107"/>
       <c r="D26" s="12"/>
     </row>
     <row r="27" spans="2:4" ht="18" x14ac:dyDescent="0.35">
-      <c r="B27" s="112"/>
-      <c r="C27" s="112"/>
-      <c r="D27" s="113"/>
+      <c r="B27" s="108"/>
+      <c r="C27" s="108"/>
+      <c r="D27" s="109"/>
     </row>
     <row r="28" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B28" s="1" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="C28" s="2"/>
       <c r="D28" s="3"/>
     </row>
     <row r="29" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B29" s="78" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="C29" s="65"/>
       <c r="D29" s="12"/>
     </row>
     <row r="30" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B30" s="98" t="s">
-        <v>229</v>
-      </c>
-      <c r="C30" s="99"/>
+      <c r="B30" s="106" t="s">
+        <v>226</v>
+      </c>
+      <c r="C30" s="107"/>
       <c r="D30" s="12"/>
     </row>
     <row r="31" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B31" s="98" t="s">
+      <c r="B31" s="106" t="s">
         <v>89</v>
       </c>
-      <c r="C31" s="99"/>
+      <c r="C31" s="107"/>
       <c r="D31" s="12"/>
     </row>
     <row r="32" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B32" s="98" t="s">
+      <c r="B32" s="106" t="s">
         <v>64</v>
       </c>
-      <c r="C32" s="99"/>
+      <c r="C32" s="107"/>
       <c r="D32" s="12"/>
     </row>
     <row r="33" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B33" s="98" t="s">
-        <v>230</v>
-      </c>
-      <c r="C33" s="99"/>
+      <c r="B33" s="106" t="s">
+        <v>227</v>
+      </c>
+      <c r="C33" s="107"/>
       <c r="D33" s="12"/>
     </row>
     <row r="34" spans="2:4" ht="18" x14ac:dyDescent="0.35">
-      <c r="B34" s="112"/>
-      <c r="C34" s="112"/>
-      <c r="D34" s="113"/>
+      <c r="B34" s="108"/>
+      <c r="C34" s="108"/>
+      <c r="D34" s="109"/>
     </row>
     <row r="35" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B35" s="1" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="C35" s="2"/>
       <c r="D35" s="3"/>
     </row>
     <row r="36" spans="2:4" ht="18" x14ac:dyDescent="0.25">
-      <c r="B36" s="114"/>
-      <c r="C36" s="115"/>
-      <c r="D36" s="116"/>
+      <c r="B36" s="103"/>
+      <c r="C36" s="104"/>
+      <c r="D36" s="105"/>
     </row>
     <row r="37" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B37" s="100" t="s">
+      <c r="B37" s="101" t="s">
+        <v>119</v>
+      </c>
+      <c r="C37" s="102"/>
+      <c r="D37" s="56"/>
+    </row>
+    <row r="38" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B38" s="101" t="s">
+        <v>120</v>
+      </c>
+      <c r="C38" s="102"/>
+      <c r="D38" s="56"/>
+    </row>
+    <row r="39" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B39" s="101" t="s">
         <v>121</v>
       </c>
-      <c r="C37" s="117"/>
-      <c r="D37" s="56"/>
-    </row>
-    <row r="38" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B38" s="100" t="s">
+      <c r="C39" s="102"/>
+      <c r="D39" s="56"/>
+    </row>
+    <row r="40" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B40" s="101" t="s">
+        <v>229</v>
+      </c>
+      <c r="C40" s="102"/>
+      <c r="D40" s="57"/>
+    </row>
+    <row r="41" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B41" s="101" t="s">
         <v>122</v>
       </c>
-      <c r="C38" s="117"/>
-      <c r="D38" s="56"/>
-    </row>
-    <row r="39" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B39" s="100" t="s">
-        <v>123</v>
-      </c>
-      <c r="C39" s="117"/>
-      <c r="D39" s="56"/>
-    </row>
-    <row r="40" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B40" s="100" t="s">
-        <v>232</v>
-      </c>
-      <c r="C40" s="117"/>
-      <c r="D40" s="57"/>
-    </row>
-    <row r="41" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B41" s="100" t="s">
-        <v>124</v>
-      </c>
-      <c r="C41" s="117"/>
+      <c r="C41" s="102"/>
       <c r="D41" s="56"/>
     </row>
     <row r="42" spans="2:4" ht="18" x14ac:dyDescent="0.25">
-      <c r="B42" s="114"/>
-      <c r="C42" s="115"/>
-      <c r="D42" s="116"/>
+      <c r="B42" s="103"/>
+      <c r="C42" s="104"/>
+      <c r="D42" s="105"/>
     </row>
     <row r="43" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B43" s="100" t="s">
+      <c r="B43" s="101" t="s">
+        <v>119</v>
+      </c>
+      <c r="C43" s="102"/>
+      <c r="D43" s="56"/>
+    </row>
+    <row r="44" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B44" s="101" t="s">
+        <v>120</v>
+      </c>
+      <c r="C44" s="102"/>
+      <c r="D44" s="56"/>
+    </row>
+    <row r="45" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B45" s="101" t="s">
         <v>121</v>
       </c>
-      <c r="C43" s="117"/>
-      <c r="D43" s="56"/>
-    </row>
-    <row r="44" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B44" s="100" t="s">
+      <c r="C45" s="102"/>
+      <c r="D45" s="56"/>
+    </row>
+    <row r="46" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B46" s="101" t="s">
+        <v>229</v>
+      </c>
+      <c r="C46" s="102"/>
+      <c r="D46" s="57"/>
+    </row>
+    <row r="47" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B47" s="101" t="s">
         <v>122</v>
       </c>
-      <c r="C44" s="117"/>
-      <c r="D44" s="56"/>
-    </row>
-    <row r="45" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B45" s="100" t="s">
-        <v>123</v>
-      </c>
-      <c r="C45" s="117"/>
-      <c r="D45" s="56"/>
-    </row>
-    <row r="46" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B46" s="100" t="s">
-        <v>232</v>
-      </c>
-      <c r="C46" s="117"/>
-      <c r="D46" s="57"/>
-    </row>
-    <row r="47" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B47" s="100" t="s">
-        <v>124</v>
-      </c>
-      <c r="C47" s="117"/>
+      <c r="C47" s="102"/>
       <c r="D47" s="56"/>
     </row>
   </sheetData>
   <mergeCells count="32">
-    <mergeCell ref="B44:C44"/>
-    <mergeCell ref="B45:C45"/>
-    <mergeCell ref="B46:C46"/>
-    <mergeCell ref="B47:C47"/>
-    <mergeCell ref="B38:C38"/>
-    <mergeCell ref="B39:C39"/>
-    <mergeCell ref="B40:C40"/>
-    <mergeCell ref="B41:C41"/>
-    <mergeCell ref="B42:D42"/>
-    <mergeCell ref="B43:C43"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B2:D8"/>
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="B17:C17"/>
     <mergeCell ref="B19:C19"/>
     <mergeCell ref="B23:C23"/>
     <mergeCell ref="B36:D36"/>
@@ -3627,14 +3625,16 @@
     <mergeCell ref="B24:C24"/>
     <mergeCell ref="B25:C25"/>
     <mergeCell ref="B26:C26"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="B2:D8"/>
-    <mergeCell ref="B9:D9"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B44:C44"/>
+    <mergeCell ref="B45:C45"/>
+    <mergeCell ref="B46:C46"/>
+    <mergeCell ref="B47:C47"/>
+    <mergeCell ref="B38:C38"/>
+    <mergeCell ref="B39:C39"/>
+    <mergeCell ref="B40:C40"/>
+    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="B42:D42"/>
+    <mergeCell ref="B43:C43"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3647,8 +3647,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="B1:X50"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A13" zoomScaleNormal="100" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6:I6"/>
+    <sheetView showGridLines="0" topLeftCell="E22" zoomScaleNormal="100" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="C48" sqref="C48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -3667,7 +3667,7 @@
     <row r="2" spans="2:24" ht="16.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B2" s="7"/>
       <c r="C2" s="22" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D2" s="8"/>
       <c r="E2" s="8"/>
@@ -3681,11 +3681,11 @@
       <c r="F3" s="8"/>
     </row>
     <row r="4" spans="2:24" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="B4" s="122"/>
-      <c r="C4" s="122"/>
-      <c r="D4" s="122"/>
-      <c r="E4" s="122"/>
-      <c r="F4" s="122"/>
+      <c r="B4" s="137"/>
+      <c r="C4" s="137"/>
+      <c r="D4" s="137"/>
+      <c r="E4" s="137"/>
+      <c r="F4" s="137"/>
     </row>
     <row r="5" spans="2:24" ht="15.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B5" s="20"/>
@@ -3700,16 +3700,16 @@
       <c r="D6" s="21"/>
       <c r="E6" s="21"/>
       <c r="F6" s="21"/>
-      <c r="G6" s="132" t="s">
-        <v>216</v>
-      </c>
-      <c r="H6" s="133"/>
-      <c r="I6" s="134"/>
-      <c r="V6" s="135" t="s">
-        <v>91</v>
-      </c>
-      <c r="W6" s="136"/>
-      <c r="X6" s="137"/>
+      <c r="G6" s="138" t="s">
+        <v>213</v>
+      </c>
+      <c r="H6" s="139"/>
+      <c r="I6" s="140"/>
+      <c r="V6" s="121" t="s">
+        <v>90</v>
+      </c>
+      <c r="W6" s="122"/>
+      <c r="X6" s="123"/>
     </row>
     <row r="7" spans="2:24" ht="16.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B7" s="13"/>
@@ -3724,18 +3724,18 @@
       <c r="D8" s="20"/>
       <c r="E8" s="20"/>
       <c r="F8" s="20"/>
-      <c r="G8" s="123">
+      <c r="G8" s="124">
         <f>AVERAGE(G43:G50)*5</f>
         <v>2.5258318070818078</v>
       </c>
-      <c r="H8" s="124"/>
-      <c r="I8" s="125"/>
-      <c r="V8" s="123" t="e">
+      <c r="H8" s="125"/>
+      <c r="I8" s="126"/>
+      <c r="V8" s="124" t="e">
         <f>AVERAGE(K43:K50)*5</f>
         <v>#REF!</v>
       </c>
-      <c r="W8" s="124"/>
-      <c r="X8" s="125"/>
+      <c r="W8" s="125"/>
+      <c r="X8" s="126"/>
     </row>
     <row r="9" spans="2:24" ht="90.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B9" s="21"/>
@@ -3743,12 +3743,12 @@
       <c r="D9" s="21"/>
       <c r="E9" s="21"/>
       <c r="F9" s="21"/>
-      <c r="G9" s="126"/>
-      <c r="H9" s="127"/>
-      <c r="I9" s="128"/>
-      <c r="V9" s="126"/>
-      <c r="W9" s="127"/>
-      <c r="X9" s="128"/>
+      <c r="G9" s="127"/>
+      <c r="H9" s="128"/>
+      <c r="I9" s="129"/>
+      <c r="V9" s="127"/>
+      <c r="W9" s="128"/>
+      <c r="X9" s="129"/>
     </row>
     <row r="10" spans="2:24" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B10" s="13"/>
@@ -3756,12 +3756,12 @@
       <c r="D10" s="13"/>
       <c r="E10" s="13"/>
       <c r="F10" s="13"/>
-      <c r="G10" s="126"/>
-      <c r="H10" s="127"/>
-      <c r="I10" s="128"/>
-      <c r="V10" s="126"/>
-      <c r="W10" s="127"/>
-      <c r="X10" s="128"/>
+      <c r="G10" s="127"/>
+      <c r="H10" s="128"/>
+      <c r="I10" s="129"/>
+      <c r="V10" s="127"/>
+      <c r="W10" s="128"/>
+      <c r="X10" s="129"/>
     </row>
     <row r="11" spans="2:24" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B11" s="13"/>
@@ -3769,19 +3769,19 @@
       <c r="D11" s="13"/>
       <c r="E11" s="13"/>
       <c r="F11" s="13"/>
-      <c r="G11" s="129"/>
-      <c r="H11" s="130"/>
-      <c r="I11" s="131"/>
-      <c r="V11" s="129"/>
-      <c r="W11" s="130"/>
-      <c r="X11" s="131"/>
+      <c r="G11" s="130"/>
+      <c r="H11" s="131"/>
+      <c r="I11" s="132"/>
+      <c r="V11" s="130"/>
+      <c r="W11" s="131"/>
+      <c r="X11" s="132"/>
     </row>
     <row r="12" spans="2:24" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B12" s="118"/>
-      <c r="C12" s="118"/>
-      <c r="D12" s="118"/>
-      <c r="E12" s="118"/>
-      <c r="F12" s="118"/>
+      <c r="B12" s="133"/>
+      <c r="C12" s="133"/>
+      <c r="D12" s="133"/>
+      <c r="E12" s="133"/>
+      <c r="F12" s="133"/>
     </row>
     <row r="13" spans="2:24" ht="15" x14ac:dyDescent="0.2">
       <c r="B13" s="14"/>
@@ -3805,11 +3805,11 @@
       <c r="F15" s="13"/>
     </row>
     <row r="16" spans="2:24" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B16" s="118"/>
-      <c r="C16" s="118"/>
-      <c r="D16" s="118"/>
-      <c r="E16" s="118"/>
-      <c r="F16" s="118"/>
+      <c r="B16" s="133"/>
+      <c r="C16" s="133"/>
+      <c r="D16" s="133"/>
+      <c r="E16" s="133"/>
+      <c r="F16" s="133"/>
     </row>
     <row r="17" spans="2:6" ht="15" x14ac:dyDescent="0.2">
       <c r="B17" s="14"/>
@@ -3862,18 +3862,18 @@
     </row>
     <row r="35" spans="3:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="41" spans="3:11" ht="16.5" x14ac:dyDescent="0.2">
-      <c r="D41" s="119" t="s">
+      <c r="D41" s="134" t="s">
         <v>71</v>
       </c>
-      <c r="E41" s="120"/>
-      <c r="F41" s="120"/>
-      <c r="G41" s="121"/>
-      <c r="H41" s="119" t="s">
+      <c r="E41" s="135"/>
+      <c r="F41" s="135"/>
+      <c r="G41" s="136"/>
+      <c r="H41" s="134" t="s">
         <v>72</v>
       </c>
-      <c r="I41" s="120"/>
-      <c r="J41" s="120"/>
-      <c r="K41" s="121"/>
+      <c r="I41" s="135"/>
+      <c r="J41" s="135"/>
+      <c r="K41" s="136"/>
     </row>
     <row r="42" spans="3:11" x14ac:dyDescent="0.2">
       <c r="D42" s="17" t="s">
@@ -3903,7 +3903,7 @@
     </row>
     <row r="43" spans="3:11" ht="16.5" x14ac:dyDescent="0.2">
       <c r="C43" s="11" t="s">
-        <v>90</v>
+        <v>255</v>
       </c>
       <c r="D43" s="9">
         <v>5</v>
@@ -3938,7 +3938,7 @@
     </row>
     <row r="44" spans="3:11" ht="16.5" x14ac:dyDescent="0.2">
       <c r="C44" s="11" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="D44" s="9">
         <v>5</v>
@@ -3973,7 +3973,7 @@
     </row>
     <row r="45" spans="3:11" ht="16.5" x14ac:dyDescent="0.2">
       <c r="C45" s="11" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="D45" s="9">
         <v>3</v>
@@ -4008,7 +4008,7 @@
     </row>
     <row r="46" spans="3:11" ht="16.5" x14ac:dyDescent="0.2">
       <c r="C46" s="11" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D46" s="9">
         <v>2</v>
@@ -4043,7 +4043,7 @@
     </row>
     <row r="47" spans="3:11" ht="16.5" x14ac:dyDescent="0.2">
       <c r="C47" s="11" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="D47" s="9">
         <v>4</v>
@@ -4078,7 +4078,7 @@
     </row>
     <row r="48" spans="3:11" ht="16.5" x14ac:dyDescent="0.2">
       <c r="C48" s="11" t="s">
-        <v>215</v>
+        <v>258</v>
       </c>
       <c r="D48" s="9">
         <v>6</v>
@@ -4113,7 +4113,7 @@
     </row>
     <row r="49" spans="3:11" ht="16.5" x14ac:dyDescent="0.2">
       <c r="C49" s="11" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="D49" s="9">
         <v>6</v>
@@ -4148,7 +4148,7 @@
     </row>
     <row r="50" spans="3:11" ht="16.5" x14ac:dyDescent="0.2">
       <c r="C50" s="11" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D50" s="9">
         <v>5</v>
@@ -4183,15 +4183,15 @@
     </row>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="B4:F4"/>
+    <mergeCell ref="G8:I11"/>
+    <mergeCell ref="G6:I6"/>
     <mergeCell ref="V6:X6"/>
     <mergeCell ref="V8:X11"/>
     <mergeCell ref="B12:F12"/>
     <mergeCell ref="B16:F16"/>
     <mergeCell ref="D41:G41"/>
     <mergeCell ref="H41:K41"/>
-    <mergeCell ref="B4:F4"/>
-    <mergeCell ref="G8:I11"/>
-    <mergeCell ref="G6:I6"/>
   </mergeCells>
   <conditionalFormatting sqref="F14">
     <cfRule type="iconSet" priority="3">
@@ -4233,7 +4233,7 @@
   <dimension ref="B1:J85"/>
   <sheetViews>
     <sheetView showGridLines="0" topLeftCell="A58" zoomScale="78" zoomScaleNormal="78" zoomScalePageLayoutView="130" workbookViewId="0">
-      <selection activeCell="G70" sqref="G70"/>
+      <selection activeCell="F68" sqref="F68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -4250,15 +4250,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:8" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B1" s="138" t="s">
-        <v>133</v>
-      </c>
-      <c r="C1" s="138"/>
-      <c r="D1" s="138"/>
-      <c r="E1" s="138"/>
-      <c r="F1" s="138"/>
-      <c r="G1" s="138"/>
-      <c r="H1" s="138"/>
+      <c r="B1" s="141" t="s">
+        <v>131</v>
+      </c>
+      <c r="C1" s="141"/>
+      <c r="D1" s="141"/>
+      <c r="E1" s="141"/>
+      <c r="F1" s="141"/>
+      <c r="G1" s="141"/>
+      <c r="H1" s="141"/>
     </row>
     <row r="2" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B2" s="45"/>
@@ -4274,22 +4274,22 @@
         <v>0</v>
       </c>
       <c r="C3" s="81" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="D3" s="26" t="s">
+        <v>94</v>
+      </c>
+      <c r="E3" s="26" t="s">
         <v>95</v>
       </c>
-      <c r="E3" s="26" t="s">
+      <c r="F3" s="26" t="s">
         <v>96</v>
       </c>
-      <c r="F3" s="26" t="s">
-        <v>97</v>
-      </c>
       <c r="G3" s="82" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="H3" s="83" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
@@ -4297,7 +4297,7 @@
         <v>1</v>
       </c>
       <c r="C4" s="28" t="s">
-        <v>98</v>
+        <v>256</v>
       </c>
       <c r="D4" s="29"/>
       <c r="E4" s="29"/>
@@ -4310,7 +4310,7 @@
         <v>2</v>
       </c>
       <c r="C5" s="32" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="D5" s="24" t="s">
         <v>3</v>
@@ -4329,7 +4329,7 @@
         <v>1.2</v>
       </c>
       <c r="C6" s="32" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="D6" s="24" t="s">
         <v>3</v>
@@ -4348,7 +4348,7 @@
         <v>1.3</v>
       </c>
       <c r="C7" s="32" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="D7" s="24" t="s">
         <v>3</v>
@@ -4367,7 +4367,7 @@
         <v>1.4</v>
       </c>
       <c r="C8" s="32" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D8" s="24" t="s">
         <v>3</v>
@@ -4386,7 +4386,7 @@
         <v>1.5</v>
       </c>
       <c r="C9" s="32" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D9" s="32"/>
       <c r="E9" s="46" t="s">
@@ -4405,7 +4405,7 @@
         <v>1.6</v>
       </c>
       <c r="C10" s="32" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="D10" s="32"/>
       <c r="E10" s="46" t="s">
@@ -4424,7 +4424,7 @@
         <v>4</v>
       </c>
       <c r="C11" s="32" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="D11" s="48"/>
       <c r="E11" s="46" t="s">
@@ -4443,7 +4443,7 @@
         <v>1.8</v>
       </c>
       <c r="C12" s="32" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="D12" s="32"/>
       <c r="E12" s="46" t="s">
@@ -4462,7 +4462,7 @@
         <v>1.9</v>
       </c>
       <c r="C13" s="32" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="D13" s="32"/>
       <c r="E13" s="46" t="s">
@@ -4481,7 +4481,7 @@
         <v>5</v>
       </c>
       <c r="C14" s="32" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="D14" s="32"/>
       <c r="E14" s="46" t="s">
@@ -4500,7 +4500,7 @@
         <v>6</v>
       </c>
       <c r="C15" s="35" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="D15" s="35"/>
       <c r="E15" s="49"/>
@@ -4513,7 +4513,7 @@
         <v>7</v>
       </c>
       <c r="C16" s="51" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="D16" s="24" t="s">
         <v>3</v>
@@ -4533,7 +4533,7 @@
         <v>39</v>
       </c>
       <c r="C17" s="51" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D17" s="24"/>
       <c r="E17" s="46"/>
@@ -4549,7 +4549,7 @@
         <v>40</v>
       </c>
       <c r="C18" s="51" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="D18" s="24" t="s">
         <v>3</v>
@@ -4569,7 +4569,7 @@
         <v>8</v>
       </c>
       <c r="C19" s="51" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="D19" s="24" t="s">
         <v>3</v>
@@ -4589,7 +4589,7 @@
         <v>41</v>
       </c>
       <c r="C20" s="51" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="D20" s="24" t="s">
         <v>3</v>
@@ -4609,7 +4609,7 @@
         <v>9</v>
       </c>
       <c r="C21" s="51" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="D21" s="24" t="s">
         <v>3</v>
@@ -4629,7 +4629,7 @@
         <v>10</v>
       </c>
       <c r="C22" s="51" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="D22" s="24" t="s">
         <v>3</v>
@@ -4649,7 +4649,7 @@
         <v>11</v>
       </c>
       <c r="C23" s="51" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="D23" s="51"/>
       <c r="E23" s="46" t="s">
@@ -4669,7 +4669,7 @@
         <v>12</v>
       </c>
       <c r="C24" s="51" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="D24" s="51"/>
       <c r="E24" s="46" t="s">
@@ -4689,7 +4689,7 @@
         <v>42</v>
       </c>
       <c r="C25" s="51" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="D25" s="51"/>
       <c r="E25" s="46" t="s">
@@ -4709,7 +4709,7 @@
         <v>43</v>
       </c>
       <c r="C26" s="51" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="D26" s="51"/>
       <c r="E26" s="46" t="s">
@@ -4729,7 +4729,7 @@
         <v>13</v>
       </c>
       <c r="C27" s="51" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="D27" s="51"/>
       <c r="E27" s="46" t="s">
@@ -4746,7 +4746,7 @@
         <v>14</v>
       </c>
       <c r="C28" s="35" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D28" s="35"/>
       <c r="E28" s="49"/>
@@ -4759,7 +4759,7 @@
         <v>15</v>
       </c>
       <c r="C29" s="51" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="D29" s="24" t="s">
         <v>3</v>
@@ -4779,7 +4779,7 @@
         <v>16</v>
       </c>
       <c r="C30" s="51" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="D30" s="24" t="s">
         <v>3</v>
@@ -4799,7 +4799,7 @@
         <v>17</v>
       </c>
       <c r="C31" s="51" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="D31" s="24" t="s">
         <v>3</v>
@@ -4819,7 +4819,7 @@
         <v>18</v>
       </c>
       <c r="C32" s="51" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="D32" s="24" t="s">
         <v>3</v>
@@ -4839,7 +4839,7 @@
         <v>19</v>
       </c>
       <c r="C33" s="51" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="D33" s="24" t="s">
         <v>3</v>
@@ -4859,7 +4859,7 @@
         <v>20</v>
       </c>
       <c r="C34" s="51" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="D34" s="24" t="s">
         <v>3</v>
@@ -4879,7 +4879,7 @@
         <v>21</v>
       </c>
       <c r="C35" s="35" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D35" s="35"/>
       <c r="E35" s="49"/>
@@ -4892,7 +4892,7 @@
         <v>22</v>
       </c>
       <c r="C36" s="51" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="D36" s="24" t="s">
         <v>3</v>
@@ -4912,7 +4912,7 @@
         <v>44</v>
       </c>
       <c r="C37" s="51" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="D37" s="24" t="s">
         <v>3</v>
@@ -4932,7 +4932,7 @@
         <v>45</v>
       </c>
       <c r="C38" s="51" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="D38" s="24" t="s">
         <v>3</v>
@@ -4953,7 +4953,7 @@
         <v>23</v>
       </c>
       <c r="C39" s="51" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="D39" s="24"/>
       <c r="E39" s="46"/>
@@ -4970,7 +4970,7 @@
         <v>24</v>
       </c>
       <c r="C40" s="51" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="D40" s="24" t="s">
         <v>3</v>
@@ -4990,7 +4990,7 @@
         <v>46</v>
       </c>
       <c r="C41" s="51" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D41" s="24" t="s">
         <v>3</v>
@@ -5010,7 +5010,7 @@
         <v>47</v>
       </c>
       <c r="C42" s="51" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="D42" s="24" t="s">
         <v>3</v>
@@ -5030,7 +5030,7 @@
         <v>25</v>
       </c>
       <c r="C43" s="51" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="D43" s="51"/>
       <c r="E43" s="46" t="s">
@@ -5050,7 +5050,7 @@
         <v>26</v>
       </c>
       <c r="C44" s="51" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="D44" s="51"/>
       <c r="E44" s="46" t="s">
@@ -5070,7 +5070,7 @@
         <v>27</v>
       </c>
       <c r="C45" s="51" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="D45" s="51"/>
       <c r="E45" s="46" t="s">
@@ -5090,7 +5090,7 @@
         <v>81</v>
       </c>
       <c r="C46" s="51" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="D46" s="51"/>
       <c r="E46" s="46" t="s">
@@ -5110,7 +5110,7 @@
         <v>28</v>
       </c>
       <c r="C47" s="35" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D47" s="35"/>
       <c r="E47" s="49"/>
@@ -5123,7 +5123,7 @@
         <v>29</v>
       </c>
       <c r="C48" s="51" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D48" s="24" t="s">
         <v>3</v>
@@ -5143,7 +5143,7 @@
         <v>48</v>
       </c>
       <c r="C49" s="51" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="D49" s="24" t="s">
         <v>3</v>
@@ -5163,7 +5163,7 @@
         <v>30</v>
       </c>
       <c r="C50" s="51" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="D50" s="24" t="s">
         <v>3</v>
@@ -5183,7 +5183,7 @@
         <v>49</v>
       </c>
       <c r="C51" s="51" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="D51" s="51"/>
       <c r="E51" s="46" t="s">
@@ -5203,7 +5203,7 @@
         <v>31</v>
       </c>
       <c r="C52" s="51" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="D52" s="51"/>
       <c r="E52" s="46" t="s">
@@ -5223,7 +5223,7 @@
         <v>5.6</v>
       </c>
       <c r="C53" s="51" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="D53" s="51"/>
       <c r="E53" s="46" t="s">
@@ -5243,7 +5243,7 @@
         <v>32</v>
       </c>
       <c r="C54" s="35" t="s">
-        <v>234</v>
+        <v>257</v>
       </c>
       <c r="D54" s="35"/>
       <c r="E54" s="49"/>
@@ -5256,7 +5256,7 @@
         <v>50</v>
       </c>
       <c r="C55" s="51" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="D55" s="24" t="s">
         <v>3</v>
@@ -5276,7 +5276,7 @@
         <v>51</v>
       </c>
       <c r="C56" s="51" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D56" s="24" t="s">
         <v>3</v>
@@ -5296,7 +5296,7 @@
         <v>52</v>
       </c>
       <c r="C57" s="51" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="D57" s="24" t="s">
         <v>3</v>
@@ -5316,7 +5316,7 @@
         <v>53</v>
       </c>
       <c r="C58" s="51" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="D58" s="24" t="s">
         <v>3</v>
@@ -5336,7 +5336,7 @@
         <v>54</v>
       </c>
       <c r="C59" s="51" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="D59" s="24" t="s">
         <v>3</v>
@@ -5356,7 +5356,7 @@
         <v>55</v>
       </c>
       <c r="C60" s="51" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="D60" s="24" t="s">
         <v>3</v>
@@ -5376,7 +5376,7 @@
         <v>83</v>
       </c>
       <c r="C61" s="51" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="D61" s="24" t="s">
         <v>3</v>
@@ -5396,7 +5396,7 @@
         <v>6.8</v>
       </c>
       <c r="C62" s="51" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="D62" s="24" t="s">
         <v>3</v>
@@ -5416,7 +5416,7 @@
         <v>33</v>
       </c>
       <c r="C63" s="35" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="D63" s="35"/>
       <c r="E63" s="49"/>
@@ -5429,7 +5429,7 @@
         <v>56</v>
       </c>
       <c r="C64" s="51" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="D64" s="24" t="s">
         <v>3</v>
@@ -5449,7 +5449,7 @@
         <v>34</v>
       </c>
       <c r="C65" s="51" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="D65" s="24" t="s">
         <v>3</v>
@@ -5469,7 +5469,7 @@
         <v>57</v>
       </c>
       <c r="C66" s="51" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="D66" s="24" t="s">
         <v>3</v>
@@ -5489,7 +5489,7 @@
         <v>58</v>
       </c>
       <c r="C67" s="51" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="D67" s="24" t="s">
         <v>3</v>
@@ -5509,7 +5509,7 @@
         <v>59</v>
       </c>
       <c r="C68" s="51" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="D68" s="24" t="s">
         <v>3</v>
@@ -5519,7 +5519,7 @@
       </c>
       <c r="F68" s="33"/>
       <c r="G68" s="52" t="s">
-        <v>253</v>
+        <v>248</v>
       </c>
       <c r="H68" s="66"/>
     </row>
@@ -5528,7 +5528,7 @@
         <v>35</v>
       </c>
       <c r="C69" s="51" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D69" s="24" t="s">
         <v>3</v>
@@ -5548,7 +5548,7 @@
         <v>36</v>
       </c>
       <c r="C70" s="51" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="D70" s="24" t="s">
         <v>3</v>
@@ -5558,7 +5558,7 @@
       </c>
       <c r="F70" s="33"/>
       <c r="G70" s="95" t="s">
-        <v>254</v>
+        <v>249</v>
       </c>
       <c r="H70" s="66"/>
     </row>
@@ -5567,7 +5567,7 @@
         <v>37</v>
       </c>
       <c r="C71" s="51" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="D71" s="24" t="s">
         <v>3</v>
@@ -5587,7 +5587,7 @@
         <v>82</v>
       </c>
       <c r="C72" s="51" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="D72" s="24" t="s">
         <v>3</v>
@@ -5640,7 +5640,7 @@
     </row>
     <row r="77" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B77" s="85" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="C77" s="42"/>
       <c r="D77" s="41"/>
@@ -5651,10 +5651,10 @@
     </row>
     <row r="78" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B78" s="87" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="C78" s="43" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="D78" s="41"/>
       <c r="E78" s="41"/>
@@ -5664,10 +5664,10 @@
     </row>
     <row r="79" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B79" s="86" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="C79" s="86" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="D79" s="41"/>
       <c r="E79" s="41"/>
@@ -5677,10 +5677,10 @@
     </row>
     <row r="80" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B80" s="86" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="C80" s="44" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D80" s="41"/>
       <c r="E80" s="41"/>
@@ -5693,7 +5693,7 @@
         <v>63</v>
       </c>
       <c r="C81" s="86" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="D81" s="41"/>
       <c r="E81" s="41"/>
@@ -5746,7 +5746,7 @@
       <formula1>"Yes,No,N/A"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F16:F27 F5:F14 F29:F34 F36:F46 F48:F53 F55:F62 F64:F72" xr:uid="{00000000-0002-0000-0200-000001000000}">
-      <formula1>"Succès,Echec,N/A"</formula1>
+      <formula1>$B$79:$B$81</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
@@ -5762,8 +5762,8 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="B1:G29"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="C4" zoomScale="91" zoomScaleNormal="91" zoomScalePageLayoutView="130" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView showGridLines="0" zoomScale="91" zoomScaleNormal="91" zoomScalePageLayoutView="130" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -5779,7 +5779,7 @@
   <sheetData>
     <row r="1" spans="2:7" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B1" s="6" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C1" s="23"/>
       <c r="D1" s="23"/>
@@ -5798,25 +5798,25 @@
     <row r="3" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B3" s="68"/>
       <c r="C3" s="69" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D3" s="68" t="s">
         <v>38</v>
       </c>
       <c r="E3" s="84" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F3" s="84" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="G3" s="84" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
     </row>
     <row r="4" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B4" s="70"/>
       <c r="C4" s="71" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="D4" s="71"/>
       <c r="E4" s="71"/>
@@ -5828,7 +5828,7 @@
         <v>8.1</v>
       </c>
       <c r="C5" s="73" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="D5" s="74" t="s">
         <v>3</v>
@@ -5847,7 +5847,7 @@
         <v>8.1999999999999993</v>
       </c>
       <c r="C6" s="73" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="D6" s="74" t="s">
         <v>3</v>
@@ -5866,7 +5866,7 @@
         <v>8.3000000000000007</v>
       </c>
       <c r="C7" s="73" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="D7" s="74" t="s">
         <v>3</v>
@@ -5885,7 +5885,7 @@
         <v>8.4</v>
       </c>
       <c r="C8" s="73" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="D8" s="74" t="s">
         <v>3</v>
@@ -5904,7 +5904,7 @@
         <v>8.5</v>
       </c>
       <c r="C9" s="73" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="D9" s="74" t="s">
         <v>3</v>
@@ -5923,7 +5923,7 @@
         <v>8.6</v>
       </c>
       <c r="C10" s="73" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="D10" s="74" t="s">
         <v>3</v>
@@ -5942,7 +5942,7 @@
         <v>8.6999999999999993</v>
       </c>
       <c r="C11" s="73" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="D11" s="74" t="s">
         <v>3</v>
@@ -5958,7 +5958,7 @@
         <v>8.8000000000000007</v>
       </c>
       <c r="C12" s="73" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="D12" s="74" t="s">
         <v>3</v>
@@ -5974,7 +5974,7 @@
         <v>8.9</v>
       </c>
       <c r="C13" s="73" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="D13" s="74" t="s">
         <v>3</v>
@@ -5991,7 +5991,7 @@
     <row r="14" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B14" s="70"/>
       <c r="C14" s="71" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D14" s="71"/>
       <c r="E14" s="71"/>
@@ -6003,7 +6003,7 @@
         <v>60</v>
       </c>
       <c r="C15" s="73" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="D15" s="74" t="s">
         <v>3</v>
@@ -6020,7 +6020,7 @@
     <row r="16" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B16" s="70"/>
       <c r="C16" s="71" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="D16" s="71"/>
       <c r="E16" s="71"/>
@@ -6032,7 +6032,7 @@
         <v>8.11</v>
       </c>
       <c r="C17" s="73" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="D17" s="74" t="s">
         <v>3</v>
@@ -6048,7 +6048,7 @@
         <v>8.1199999999999992</v>
       </c>
       <c r="C18" s="73" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="D18" s="74" t="s">
         <v>3</v>
@@ -6085,7 +6085,7 @@
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B22" s="85" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="C22" s="42"/>
       <c r="D22" s="41"/>
@@ -6095,10 +6095,10 @@
     </row>
     <row r="23" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B23" s="87" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="C23" s="43" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="D23" s="41"/>
       <c r="E23" s="41"/>
@@ -6107,10 +6107,10 @@
     </row>
     <row r="24" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B24" s="86" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="C24" s="86" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="D24" s="41"/>
       <c r="E24" s="41"/>
@@ -6119,10 +6119,10 @@
     </row>
     <row r="25" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B25" s="86" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="C25" s="44" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D25" s="41"/>
       <c r="E25" s="41"/>
@@ -6134,7 +6134,7 @@
         <v>63</v>
       </c>
       <c r="C26" s="86" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="D26" s="41"/>
       <c r="E26" s="41"/>
@@ -6168,7 +6168,7 @@
   </sheetData>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E17:E18 E15 E5:E13" xr:uid="{00000000-0002-0000-0300-000000000000}">
-      <formula1>"Pass,Fail,N/A"</formula1>
+      <formula1>$B$24:$B$26</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -6180,8 +6180,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="B1:J85"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A67" zoomScale="78" zoomScaleNormal="78" zoomScalePageLayoutView="130" workbookViewId="0">
-      <selection activeCell="G70" sqref="G70"/>
+    <sheetView showGridLines="0" topLeftCell="A46" zoomScale="78" zoomScaleNormal="78" zoomScalePageLayoutView="130" workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -6198,15 +6198,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:8" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B1" s="138" t="s">
-        <v>212</v>
-      </c>
-      <c r="C1" s="138"/>
-      <c r="D1" s="138"/>
-      <c r="E1" s="138"/>
-      <c r="F1" s="138"/>
-      <c r="G1" s="138"/>
-      <c r="H1" s="138"/>
+      <c r="B1" s="141" t="s">
+        <v>210</v>
+      </c>
+      <c r="C1" s="141"/>
+      <c r="D1" s="141"/>
+      <c r="E1" s="141"/>
+      <c r="F1" s="141"/>
+      <c r="G1" s="141"/>
+      <c r="H1" s="141"/>
     </row>
     <row r="2" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B2" s="45"/>
@@ -6222,22 +6222,22 @@
         <v>0</v>
       </c>
       <c r="C3" s="81" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="D3" s="26" t="s">
+        <v>94</v>
+      </c>
+      <c r="E3" s="26" t="s">
         <v>95</v>
       </c>
-      <c r="E3" s="26" t="s">
+      <c r="F3" s="26" t="s">
         <v>96</v>
       </c>
-      <c r="F3" s="26" t="s">
-        <v>97</v>
-      </c>
       <c r="G3" s="82" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="H3" s="83" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
@@ -6245,7 +6245,7 @@
         <v>1</v>
       </c>
       <c r="C4" s="28" t="s">
-        <v>98</v>
+        <v>256</v>
       </c>
       <c r="D4" s="29"/>
       <c r="E4" s="29"/>
@@ -6258,7 +6258,7 @@
         <v>2</v>
       </c>
       <c r="C5" s="32" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="D5" s="24" t="s">
         <v>3</v>
@@ -6277,7 +6277,7 @@
         <v>1.2</v>
       </c>
       <c r="C6" s="32" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="D6" s="24" t="s">
         <v>3</v>
@@ -6296,7 +6296,7 @@
         <v>1.3</v>
       </c>
       <c r="C7" s="32" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="D7" s="24" t="s">
         <v>3</v>
@@ -6315,7 +6315,7 @@
         <v>1.4</v>
       </c>
       <c r="C8" s="32" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D8" s="24" t="s">
         <v>3</v>
@@ -6334,7 +6334,7 @@
         <v>1.5</v>
       </c>
       <c r="C9" s="32" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D9" s="32"/>
       <c r="E9" s="46" t="s">
@@ -6353,7 +6353,7 @@
         <v>1.6</v>
       </c>
       <c r="C10" s="32" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="D10" s="32"/>
       <c r="E10" s="46" t="s">
@@ -6372,7 +6372,7 @@
         <v>4</v>
       </c>
       <c r="C11" s="32" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="D11" s="48"/>
       <c r="E11" s="46" t="s">
@@ -6391,7 +6391,7 @@
         <v>1.8</v>
       </c>
       <c r="C12" s="32" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="D12" s="32"/>
       <c r="E12" s="46" t="s">
@@ -6410,7 +6410,7 @@
         <v>1.9</v>
       </c>
       <c r="C13" s="32" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="D13" s="32"/>
       <c r="E13" s="46" t="s">
@@ -6429,7 +6429,7 @@
         <v>5</v>
       </c>
       <c r="C14" s="32" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="D14" s="32"/>
       <c r="E14" s="46" t="s">
@@ -6448,7 +6448,7 @@
         <v>6</v>
       </c>
       <c r="C15" s="35" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="D15" s="35"/>
       <c r="E15" s="49"/>
@@ -6461,7 +6461,7 @@
         <v>7</v>
       </c>
       <c r="C16" s="51" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="D16" s="24" t="s">
         <v>3</v>
@@ -6481,7 +6481,7 @@
         <v>39</v>
       </c>
       <c r="C17" s="51" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D17" s="24"/>
       <c r="E17" s="46"/>
@@ -6497,7 +6497,7 @@
         <v>40</v>
       </c>
       <c r="C18" s="51" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="D18" s="24" t="s">
         <v>3</v>
@@ -6517,7 +6517,7 @@
         <v>8</v>
       </c>
       <c r="C19" s="51" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="D19" s="24" t="s">
         <v>3</v>
@@ -6537,7 +6537,7 @@
         <v>41</v>
       </c>
       <c r="C20" s="51" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="D20" s="24" t="s">
         <v>3</v>
@@ -6557,7 +6557,7 @@
         <v>9</v>
       </c>
       <c r="C21" s="51" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="D21" s="24" t="s">
         <v>3</v>
@@ -6577,7 +6577,7 @@
         <v>10</v>
       </c>
       <c r="C22" s="51" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="D22" s="24" t="s">
         <v>3</v>
@@ -6597,7 +6597,7 @@
         <v>11</v>
       </c>
       <c r="C23" s="51" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="D23" s="51"/>
       <c r="E23" s="46" t="s">
@@ -6617,7 +6617,7 @@
         <v>12</v>
       </c>
       <c r="C24" s="51" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="D24" s="51"/>
       <c r="E24" s="46" t="s">
@@ -6637,7 +6637,7 @@
         <v>42</v>
       </c>
       <c r="C25" s="51" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="D25" s="51"/>
       <c r="E25" s="46" t="s">
@@ -6657,7 +6657,7 @@
         <v>43</v>
       </c>
       <c r="C26" s="51" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="D26" s="51"/>
       <c r="E26" s="46" t="s">
@@ -6677,7 +6677,7 @@
         <v>13</v>
       </c>
       <c r="C27" s="51" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="D27" s="51"/>
       <c r="E27" s="46" t="s">
@@ -6694,7 +6694,7 @@
         <v>14</v>
       </c>
       <c r="C28" s="35" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D28" s="35"/>
       <c r="E28" s="49"/>
@@ -6707,7 +6707,7 @@
         <v>15</v>
       </c>
       <c r="C29" s="51" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="D29" s="24" t="s">
         <v>3</v>
@@ -6727,7 +6727,7 @@
         <v>16</v>
       </c>
       <c r="C30" s="51" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="D30" s="24" t="s">
         <v>3</v>
@@ -6747,7 +6747,7 @@
         <v>17</v>
       </c>
       <c r="C31" s="51" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="D31" s="24" t="s">
         <v>3</v>
@@ -6767,7 +6767,7 @@
         <v>18</v>
       </c>
       <c r="C32" s="51" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="D32" s="24" t="s">
         <v>3</v>
@@ -6787,7 +6787,7 @@
         <v>19</v>
       </c>
       <c r="C33" s="51" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="D33" s="24" t="s">
         <v>3</v>
@@ -6807,7 +6807,7 @@
         <v>20</v>
       </c>
       <c r="C34" s="51" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="D34" s="24" t="s">
         <v>3</v>
@@ -6827,7 +6827,7 @@
         <v>21</v>
       </c>
       <c r="C35" s="35" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D35" s="35"/>
       <c r="E35" s="49"/>
@@ -6840,7 +6840,7 @@
         <v>22</v>
       </c>
       <c r="C36" s="51" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="D36" s="24" t="s">
         <v>3</v>
@@ -6849,8 +6849,8 @@
         <v>3</v>
       </c>
       <c r="F36" s="33"/>
-      <c r="G36" s="140" t="s">
-        <v>100</v>
+      <c r="G36" s="98" t="s">
+        <v>98</v>
       </c>
       <c r="H36" s="66"/>
     </row>
@@ -6859,7 +6859,7 @@
         <v>44</v>
       </c>
       <c r="C37" s="51" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="D37" s="24" t="s">
         <v>3</v>
@@ -6868,8 +6868,8 @@
         <v>3</v>
       </c>
       <c r="F37" s="33"/>
-      <c r="G37" s="140" t="s">
-        <v>103</v>
+      <c r="G37" s="98" t="s">
+        <v>101</v>
       </c>
       <c r="H37" s="66"/>
     </row>
@@ -6878,7 +6878,7 @@
         <v>45</v>
       </c>
       <c r="C38" s="51" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="D38" s="24" t="s">
         <v>3</v>
@@ -6887,8 +6887,8 @@
         <v>3</v>
       </c>
       <c r="F38" s="33"/>
-      <c r="G38" s="140" t="s">
-        <v>102</v>
+      <c r="G38" s="98" t="s">
+        <v>100</v>
       </c>
       <c r="H38" s="66"/>
       <c r="J38" s="52"/>
@@ -6898,13 +6898,13 @@
         <v>23</v>
       </c>
       <c r="C39" s="51" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="D39" s="24"/>
       <c r="E39" s="46"/>
       <c r="F39" s="33"/>
-      <c r="G39" s="140" t="s">
-        <v>104</v>
+      <c r="G39" s="98" t="s">
+        <v>102</v>
       </c>
       <c r="H39" s="66"/>
       <c r="J39" s="52"/>
@@ -6914,7 +6914,7 @@
         <v>24</v>
       </c>
       <c r="C40" s="51" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="D40" s="24" t="s">
         <v>3</v>
@@ -6923,8 +6923,8 @@
         <v>3</v>
       </c>
       <c r="F40" s="33"/>
-      <c r="G40" s="140" t="s">
-        <v>105</v>
+      <c r="G40" s="98" t="s">
+        <v>103</v>
       </c>
       <c r="H40" s="66"/>
     </row>
@@ -6933,7 +6933,7 @@
         <v>46</v>
       </c>
       <c r="C41" s="51" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D41" s="24" t="s">
         <v>3</v>
@@ -6942,8 +6942,8 @@
         <v>3</v>
       </c>
       <c r="F41" s="33"/>
-      <c r="G41" s="140" t="s">
-        <v>106</v>
+      <c r="G41" s="98" t="s">
+        <v>104</v>
       </c>
       <c r="H41" s="66"/>
     </row>
@@ -6952,7 +6952,7 @@
         <v>47</v>
       </c>
       <c r="C42" s="51" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="D42" s="24" t="s">
         <v>3</v>
@@ -6961,8 +6961,8 @@
         <v>3</v>
       </c>
       <c r="F42" s="33"/>
-      <c r="G42" s="140" t="s">
-        <v>107</v>
+      <c r="G42" s="98" t="s">
+        <v>105</v>
       </c>
       <c r="H42" s="52"/>
     </row>
@@ -6971,7 +6971,7 @@
         <v>25</v>
       </c>
       <c r="C43" s="51" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="D43" s="51"/>
       <c r="E43" s="46" t="s">
@@ -6991,7 +6991,7 @@
         <v>26</v>
       </c>
       <c r="C44" s="51" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="D44" s="51"/>
       <c r="E44" s="46" t="s">
@@ -7000,8 +7000,8 @@
       <c r="F44" s="33" t="s">
         <v>63</v>
       </c>
-      <c r="G44" s="140" t="s">
-        <v>109</v>
+      <c r="G44" s="98" t="s">
+        <v>107</v>
       </c>
       <c r="H44" s="66"/>
     </row>
@@ -7010,7 +7010,7 @@
         <v>27</v>
       </c>
       <c r="C45" s="51" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="D45" s="51"/>
       <c r="E45" s="46" t="s">
@@ -7019,8 +7019,8 @@
       <c r="F45" s="33" t="s">
         <v>63</v>
       </c>
-      <c r="G45" s="140" t="s">
-        <v>108</v>
+      <c r="G45" s="98" t="s">
+        <v>106</v>
       </c>
       <c r="H45" s="66"/>
     </row>
@@ -7029,7 +7029,7 @@
         <v>81</v>
       </c>
       <c r="C46" s="51" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="D46" s="51"/>
       <c r="E46" s="46" t="s">
@@ -7046,7 +7046,7 @@
         <v>28</v>
       </c>
       <c r="C47" s="35" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D47" s="35"/>
       <c r="E47" s="49"/>
@@ -7059,7 +7059,7 @@
         <v>29</v>
       </c>
       <c r="C48" s="51" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D48" s="24" t="s">
         <v>3</v>
@@ -7079,7 +7079,7 @@
         <v>48</v>
       </c>
       <c r="C49" s="51" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="D49" s="24" t="s">
         <v>3</v>
@@ -7099,7 +7099,7 @@
         <v>30</v>
       </c>
       <c r="C50" s="51" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="D50" s="24" t="s">
         <v>3</v>
@@ -7119,7 +7119,7 @@
         <v>49</v>
       </c>
       <c r="C51" s="51" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="D51" s="51"/>
       <c r="E51" s="46" t="s">
@@ -7139,7 +7139,7 @@
         <v>31</v>
       </c>
       <c r="C52" s="51" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="D52" s="51"/>
       <c r="E52" s="46" t="s">
@@ -7148,8 +7148,8 @@
       <c r="F52" s="33" t="s">
         <v>63</v>
       </c>
-      <c r="G52" s="140" t="s">
-        <v>255</v>
+      <c r="G52" s="98" t="s">
+        <v>250</v>
       </c>
       <c r="H52" s="66"/>
     </row>
@@ -7158,7 +7158,7 @@
         <v>5.6</v>
       </c>
       <c r="C53" s="51" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="D53" s="51"/>
       <c r="E53" s="46" t="s">
@@ -7167,8 +7167,8 @@
       <c r="F53" s="33" t="s">
         <v>63</v>
       </c>
-      <c r="G53" s="140" t="s">
-        <v>256</v>
+      <c r="G53" s="98" t="s">
+        <v>251</v>
       </c>
       <c r="H53" s="66"/>
     </row>
@@ -7177,7 +7177,7 @@
         <v>32</v>
       </c>
       <c r="C54" s="35" t="s">
-        <v>234</v>
+        <v>257</v>
       </c>
       <c r="D54" s="35"/>
       <c r="E54" s="49"/>
@@ -7190,7 +7190,7 @@
         <v>50</v>
       </c>
       <c r="C55" s="51" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="D55" s="24" t="s">
         <v>3</v>
@@ -7210,7 +7210,7 @@
         <v>51</v>
       </c>
       <c r="C56" s="51" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D56" s="24" t="s">
         <v>3</v>
@@ -7219,8 +7219,8 @@
         <v>3</v>
       </c>
       <c r="F56" s="33"/>
-      <c r="G56" s="140" t="s">
-        <v>257</v>
+      <c r="G56" s="98" t="s">
+        <v>252</v>
       </c>
       <c r="H56" s="66"/>
     </row>
@@ -7229,7 +7229,7 @@
         <v>52</v>
       </c>
       <c r="C57" s="51" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="D57" s="24" t="s">
         <v>3</v>
@@ -7249,7 +7249,7 @@
         <v>53</v>
       </c>
       <c r="C58" s="51" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="D58" s="24" t="s">
         <v>3</v>
@@ -7258,7 +7258,7 @@
         <v>3</v>
       </c>
       <c r="F58" s="33"/>
-      <c r="G58" s="140" t="s">
+      <c r="G58" s="98" t="s">
         <v>76</v>
       </c>
       <c r="H58" s="66"/>
@@ -7268,7 +7268,7 @@
         <v>54</v>
       </c>
       <c r="C59" s="51" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="D59" s="24" t="s">
         <v>3</v>
@@ -7288,7 +7288,7 @@
         <v>55</v>
       </c>
       <c r="C60" s="51" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="D60" s="24" t="s">
         <v>3</v>
@@ -7308,7 +7308,7 @@
         <v>83</v>
       </c>
       <c r="C61" s="51" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="D61" s="24" t="s">
         <v>3</v>
@@ -7328,7 +7328,7 @@
         <v>6.8</v>
       </c>
       <c r="C62" s="51" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="D62" s="24" t="s">
         <v>3</v>
@@ -7348,7 +7348,7 @@
         <v>33</v>
       </c>
       <c r="C63" s="35" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="D63" s="35"/>
       <c r="E63" s="49"/>
@@ -7361,7 +7361,7 @@
         <v>56</v>
       </c>
       <c r="C64" s="51" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="D64" s="24" t="s">
         <v>3</v>
@@ -7381,7 +7381,7 @@
         <v>34</v>
       </c>
       <c r="C65" s="51" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="D65" s="24" t="s">
         <v>3</v>
@@ -7401,7 +7401,7 @@
         <v>57</v>
       </c>
       <c r="C66" s="51" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="D66" s="24" t="s">
         <v>3</v>
@@ -7421,7 +7421,7 @@
         <v>58</v>
       </c>
       <c r="C67" s="51" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="D67" s="24" t="s">
         <v>3</v>
@@ -7441,7 +7441,7 @@
         <v>59</v>
       </c>
       <c r="C68" s="51" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="D68" s="24" t="s">
         <v>3</v>
@@ -7451,7 +7451,7 @@
       </c>
       <c r="F68" s="33"/>
       <c r="G68" s="52" t="s">
-        <v>253</v>
+        <v>248</v>
       </c>
       <c r="H68" s="66"/>
     </row>
@@ -7460,7 +7460,7 @@
         <v>35</v>
       </c>
       <c r="C69" s="51" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D69" s="24" t="s">
         <v>3</v>
@@ -7480,7 +7480,7 @@
         <v>36</v>
       </c>
       <c r="C70" s="51" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="D70" s="24" t="s">
         <v>3</v>
@@ -7489,8 +7489,8 @@
         <v>3</v>
       </c>
       <c r="F70" s="33"/>
-      <c r="G70" s="140" t="s">
-        <v>254</v>
+      <c r="G70" s="98" t="s">
+        <v>249</v>
       </c>
       <c r="H70" s="66"/>
     </row>
@@ -7499,7 +7499,7 @@
         <v>37</v>
       </c>
       <c r="C71" s="51" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="D71" s="24" t="s">
         <v>3</v>
@@ -7508,8 +7508,8 @@
         <v>3</v>
       </c>
       <c r="F71" s="33"/>
-      <c r="G71" s="140" t="s">
-        <v>258</v>
+      <c r="G71" s="98" t="s">
+        <v>253</v>
       </c>
       <c r="H71" s="66"/>
     </row>
@@ -7518,7 +7518,7 @@
         <v>82</v>
       </c>
       <c r="C72" s="51" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="D72" s="24" t="s">
         <v>3</v>
@@ -7571,7 +7571,7 @@
     </row>
     <row r="77" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B77" s="85" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="C77" s="42"/>
       <c r="D77" s="41"/>
@@ -7582,10 +7582,10 @@
     </row>
     <row r="78" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B78" s="87" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="C78" s="43" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="D78" s="41"/>
       <c r="E78" s="41"/>
@@ -7595,10 +7595,10 @@
     </row>
     <row r="79" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B79" s="86" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="C79" s="86" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="D79" s="41"/>
       <c r="E79" s="41"/>
@@ -7608,10 +7608,10 @@
     </row>
     <row r="80" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B80" s="86" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="C80" s="44" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D80" s="41"/>
       <c r="E80" s="41"/>
@@ -7624,7 +7624,7 @@
         <v>63</v>
       </c>
       <c r="C81" s="86" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="D81" s="41"/>
       <c r="E81" s="41"/>
@@ -7674,7 +7674,7 @@
   </mergeCells>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F29:F34 F36:F46 F48:F53 F64:F72 F5:F14 F55:F62 F16:F27" xr:uid="{00000000-0002-0000-0400-000000000000}">
-      <formula1>"Pass,Fail,N/A"</formula1>
+      <formula1>$B$79:$B$81</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F74:F1048576 H74:H1048576" xr:uid="{00000000-0002-0000-0400-000001000000}">
       <formula1>"Yes,No,N/A"</formula1>
@@ -7689,8 +7689,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="B1:G29"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="71" zoomScaleNormal="71" zoomScalePageLayoutView="130" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="71" zoomScaleNormal="71" zoomScalePageLayoutView="130" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -7706,7 +7706,7 @@
   <sheetData>
     <row r="1" spans="2:7" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B1" s="6" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C1" s="23"/>
       <c r="D1" s="23"/>
@@ -7725,25 +7725,25 @@
     <row r="3" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B3" s="68"/>
       <c r="C3" s="69" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D3" s="68" t="s">
         <v>38</v>
       </c>
       <c r="E3" s="84" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F3" s="84" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="G3" s="84" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
     </row>
     <row r="4" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B4" s="70"/>
       <c r="C4" s="71" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="D4" s="71"/>
       <c r="E4" s="71"/>
@@ -7755,7 +7755,7 @@
         <v>8.1</v>
       </c>
       <c r="C5" s="73" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="D5" s="74" t="s">
         <v>3</v>
@@ -7774,7 +7774,7 @@
         <v>8.1999999999999993</v>
       </c>
       <c r="C6" s="73" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="D6" s="74" t="s">
         <v>3</v>
@@ -7782,7 +7782,7 @@
       <c r="E6" s="75" t="s">
         <v>63</v>
       </c>
-      <c r="F6" s="142" t="str">
+      <c r="F6" s="100" t="str">
         <f>HYPERLINK(CONCATENATE(BASE_URL,"0x06j-Testing-Resiliency-Against-Reverse-Engineering.md#anti-debugging-checks"),"Tester la défense contre le déboggage")</f>
         <v>Tester la défense contre le déboggage</v>
       </c>
@@ -7793,7 +7793,7 @@
         <v>8.3000000000000007</v>
       </c>
       <c r="C7" s="73" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="D7" s="74" t="s">
         <v>3</v>
@@ -7801,7 +7801,7 @@
       <c r="E7" s="75" t="s">
         <v>63</v>
       </c>
-      <c r="F7" s="142" t="str">
+      <c r="F7" s="100" t="str">
         <f>HYPERLINK(CONCATENATE(BASE_URL,"0x06j-Testing-Resiliency-Against-Reverse-Engineering.md#file-integrity-checks"),"Tester le méchanisme de vérification d'intégrité des fichiers")</f>
         <v>Tester le méchanisme de vérification d'intégrité des fichiers</v>
       </c>
@@ -7812,7 +7812,7 @@
         <v>8.4</v>
       </c>
       <c r="C8" s="73" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="D8" s="74" t="s">
         <v>3</v>
@@ -7820,7 +7820,7 @@
       <c r="E8" s="75" t="s">
         <v>63</v>
       </c>
-      <c r="F8" s="141"/>
+      <c r="F8" s="99"/>
       <c r="G8" s="73"/>
     </row>
     <row r="9" spans="2:7" x14ac:dyDescent="0.25">
@@ -7828,7 +7828,7 @@
         <v>8.5</v>
       </c>
       <c r="C9" s="73" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="D9" s="74" t="s">
         <v>3</v>
@@ -7836,7 +7836,7 @@
       <c r="E9" s="75" t="s">
         <v>63</v>
       </c>
-      <c r="F9" s="140"/>
+      <c r="F9" s="98"/>
       <c r="G9" s="73"/>
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.25">
@@ -7844,7 +7844,7 @@
         <v>8.6</v>
       </c>
       <c r="C10" s="73" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="D10" s="74" t="s">
         <v>3</v>
@@ -7852,7 +7852,7 @@
       <c r="E10" s="75" t="s">
         <v>63</v>
       </c>
-      <c r="F10" s="141"/>
+      <c r="F10" s="99"/>
       <c r="G10" s="73"/>
     </row>
     <row r="11" spans="2:7" ht="30" x14ac:dyDescent="0.25">
@@ -7860,7 +7860,7 @@
         <v>8.6999999999999993</v>
       </c>
       <c r="C11" s="73" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="D11" s="74" t="s">
         <v>3</v>
@@ -7876,7 +7876,7 @@
         <v>8.8000000000000007</v>
       </c>
       <c r="C12" s="73" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="D12" s="74" t="s">
         <v>3</v>
@@ -7892,7 +7892,7 @@
         <v>8.9</v>
       </c>
       <c r="C13" s="73" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="D13" s="74" t="s">
         <v>3</v>
@@ -7900,13 +7900,13 @@
       <c r="E13" s="75" t="s">
         <v>63</v>
       </c>
-      <c r="F13" s="140"/>
+      <c r="F13" s="98"/>
       <c r="G13" s="73"/>
     </row>
     <row r="14" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B14" s="70"/>
       <c r="C14" s="71" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D14" s="71"/>
       <c r="E14" s="71"/>
@@ -7918,7 +7918,7 @@
         <v>60</v>
       </c>
       <c r="C15" s="73" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="D15" s="74" t="s">
         <v>3</v>
@@ -7935,7 +7935,7 @@
     <row r="16" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B16" s="70"/>
       <c r="C16" s="71" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="D16" s="71"/>
       <c r="E16" s="71"/>
@@ -7947,7 +7947,7 @@
         <v>8.11</v>
       </c>
       <c r="C17" s="73" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="D17" s="74" t="s">
         <v>3</v>
@@ -7963,7 +7963,7 @@
         <v>8.1199999999999992</v>
       </c>
       <c r="C18" s="73" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="D18" s="74" t="s">
         <v>3</v>
@@ -8000,7 +8000,7 @@
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B22" s="85" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="C22" s="42"/>
       <c r="D22" s="41"/>
@@ -8010,10 +8010,10 @@
     </row>
     <row r="23" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B23" s="87" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="C23" s="43" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="D23" s="41"/>
       <c r="E23" s="41"/>
@@ -8022,10 +8022,10 @@
     </row>
     <row r="24" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B24" s="86" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="C24" s="86" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="D24" s="41"/>
       <c r="E24" s="41"/>
@@ -8034,10 +8034,10 @@
     </row>
     <row r="25" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B25" s="86" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="C25" s="44" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D25" s="41"/>
       <c r="E25" s="41"/>
@@ -8049,7 +8049,7 @@
         <v>63</v>
       </c>
       <c r="C26" s="86" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="D26" s="41"/>
       <c r="E26" s="41"/>
@@ -8081,9 +8081,12 @@
       <c r="G29" s="23"/>
     </row>
   </sheetData>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E17:E18 E15 E5:E13" xr:uid="{00000000-0002-0000-0500-000000000000}">
-      <formula1>"Pass,Fail,N/A"</formula1>
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E5:E8" xr:uid="{00000000-0002-0000-0500-000000000000}">
+      <formula1>$B$24:$B$26</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E18 E17 E15 E13 E12 E11 E10 E9" xr:uid="{26D81470-7AC7-4EC9-BAB0-839C3AE3AF8F}">
+      <formula1>$B$24:$B$26</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -8096,7 +8099,7 @@
   <sheetPr codeName="Sheet7"/>
   <dimension ref="A1:D15"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
@@ -8107,16 +8110,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="139" t="s">
-        <v>120</v>
-      </c>
-      <c r="B1" s="139"/>
+      <c r="A1" s="142" t="s">
+        <v>118</v>
+      </c>
+      <c r="B1" s="142"/>
       <c r="C1" s="45"/>
       <c r="D1" s="45"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="88" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B2" s="61" t="s">
         <v>64</v>
@@ -8125,7 +8128,7 @@
         <v>78</v>
       </c>
       <c r="D2" s="89" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -8139,7 +8142,7 @@
         <v>42765</v>
       </c>
       <c r="D3" s="58" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -8153,7 +8156,7 @@
         <v>42766</v>
       </c>
       <c r="D4" s="90" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -8167,7 +8170,7 @@
         <v>42778</v>
       </c>
       <c r="D5" s="58" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -8181,7 +8184,7 @@
         <v>42780</v>
       </c>
       <c r="D6" s="90" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -8195,7 +8198,7 @@
         <v>42781</v>
       </c>
       <c r="D7" s="58" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -8209,7 +8212,7 @@
         <v>42829</v>
       </c>
       <c r="D8" s="90" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -8223,7 +8226,7 @@
         <v>42919</v>
       </c>
       <c r="D9" s="90" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -8237,7 +8240,7 @@
         <v>42963</v>
       </c>
       <c r="D10" s="90" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -8251,7 +8254,7 @@
         <v>43113</v>
       </c>
       <c r="D11" s="90" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -8265,49 +8268,49 @@
         <v>43289</v>
       </c>
       <c r="D12" s="90" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="58" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B13" s="92" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C13" s="60">
         <v>43464</v>
       </c>
       <c r="D13" s="90" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="58" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B14" s="92" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C14" s="60">
         <v>43469</v>
       </c>
       <c r="D14" s="90" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="58" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B15" s="92" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C15" s="91">
         <v>43475</v>
       </c>
       <c r="D15" s="90" t="s">
-        <v>259</v>
+        <v>254</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Checklist French version with added missing links
</commit_message>
<xml_diff>
--- a/Checklists/Mobile_App_Security_Checklist-French.xlsx
+++ b/Checklists/Mobile_App_Security_Checklist-French.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projects\MASVS_MSTG\owasp-mstg\Checklists\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EE62FC0-003C-4393-8C21-32F4887F5D72}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2991FA44-8F6A-40F4-9DFE-8D6DDBB4A931}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6945" tabRatio="500" firstSheet="3" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6945" tabRatio="500" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tableau de Bord" sheetId="6" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="910" uniqueCount="279">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="837" uniqueCount="278">
   <si>
     <t>ID</t>
   </si>
@@ -910,9 +910,6 @@
   </si>
   <si>
     <t xml:space="preserve">                                                         -</t>
-  </si>
-  <si>
-    <t xml:space="preserve">                                                                                -</t>
   </si>
   <si>
     <t xml:space="preserve">                                                                                             -</t>
@@ -1909,7 +1906,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="176">
+  <cellXfs count="179">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
@@ -2194,148 +2191,6 @@
     <xf numFmtId="0" fontId="21" fillId="0" borderId="45" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="12" borderId="21" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="12" borderId="20" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="12" borderId="22" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="1" fontId="13" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="13" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="13" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="13" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="13" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="13" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="13" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="13" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="46" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2373,6 +2228,157 @@
     </xf>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="13" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="13" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="13" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="13" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="13" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="13" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="13" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="13" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="21" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="20" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="22" xfId="9" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="9" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="9" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="9" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="62">
@@ -3665,48 +3671,48 @@
   <sheetData>
     <row r="1" spans="2:4" ht="8.1" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B2" s="116" t="s">
+      <c r="B2" s="144" t="s">
         <v>215</v>
       </c>
-      <c r="C2" s="117"/>
-      <c r="D2" s="118"/>
+      <c r="C2" s="145"/>
+      <c r="D2" s="146"/>
     </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B3" s="119"/>
-      <c r="C3" s="120"/>
-      <c r="D3" s="121"/>
+      <c r="B3" s="147"/>
+      <c r="C3" s="148"/>
+      <c r="D3" s="149"/>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B4" s="119"/>
-      <c r="C4" s="120"/>
-      <c r="D4" s="121"/>
+      <c r="B4" s="147"/>
+      <c r="C4" s="148"/>
+      <c r="D4" s="149"/>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B5" s="119"/>
-      <c r="C5" s="120"/>
-      <c r="D5" s="121"/>
+      <c r="B5" s="147"/>
+      <c r="C5" s="148"/>
+      <c r="D5" s="149"/>
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B6" s="119"/>
-      <c r="C6" s="120"/>
-      <c r="D6" s="121"/>
+      <c r="B6" s="147"/>
+      <c r="C6" s="148"/>
+      <c r="D6" s="149"/>
     </row>
     <row r="7" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B7" s="119"/>
-      <c r="C7" s="120"/>
-      <c r="D7" s="121"/>
+      <c r="B7" s="147"/>
+      <c r="C7" s="148"/>
+      <c r="D7" s="149"/>
     </row>
     <row r="8" spans="2:4" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="122"/>
-      <c r="C8" s="123"/>
-      <c r="D8" s="124"/>
+      <c r="B8" s="150"/>
+      <c r="C8" s="151"/>
+      <c r="D8" s="152"/>
     </row>
     <row r="9" spans="2:4" ht="18" x14ac:dyDescent="0.35">
-      <c r="B9" s="125" t="s">
+      <c r="B9" s="153" t="s">
         <v>66</v>
       </c>
-      <c r="C9" s="126"/>
-      <c r="D9" s="127"/>
+      <c r="C9" s="135"/>
+      <c r="D9" s="136"/>
     </row>
     <row r="10" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
@@ -3716,10 +3722,10 @@
       <c r="D10" s="3"/>
     </row>
     <row r="11" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B11" s="112" t="s">
+      <c r="B11" s="133" t="s">
         <v>231</v>
       </c>
-      <c r="C11" s="113"/>
+      <c r="C11" s="134"/>
       <c r="D11" s="12" t="s">
         <v>232</v>
       </c>
@@ -3756,55 +3762,55 @@
       <c r="D15" s="99"/>
     </row>
     <row r="16" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B16" s="114" t="s">
+      <c r="B16" s="128" t="s">
         <v>202</v>
       </c>
-      <c r="C16" s="115"/>
+      <c r="C16" s="143"/>
       <c r="D16" s="12"/>
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B17" s="112" t="s">
+      <c r="B17" s="133" t="s">
         <v>85</v>
       </c>
-      <c r="C17" s="113"/>
+      <c r="C17" s="134"/>
       <c r="D17" s="12"/>
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B18" s="112" t="s">
+      <c r="B18" s="133" t="s">
         <v>203</v>
       </c>
-      <c r="C18" s="113"/>
+      <c r="C18" s="134"/>
       <c r="D18" s="12"/>
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B19" s="112" t="s">
+      <c r="B19" s="133" t="s">
         <v>86</v>
       </c>
-      <c r="C19" s="113"/>
+      <c r="C19" s="134"/>
       <c r="D19" s="12"/>
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B20" s="112" t="s">
+      <c r="B20" s="133" t="s">
         <v>204</v>
       </c>
-      <c r="C20" s="113"/>
+      <c r="C20" s="134"/>
       <c r="D20" s="12" t="s">
         <v>205</v>
       </c>
     </row>
     <row r="21" spans="2:4" ht="70.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="112" t="s">
+      <c r="B21" s="133" t="s">
         <v>206</v>
       </c>
-      <c r="C21" s="113"/>
+      <c r="C21" s="134"/>
       <c r="D21" s="12" t="s">
         <v>207</v>
       </c>
     </row>
     <row r="22" spans="2:4" ht="18" x14ac:dyDescent="0.35">
-      <c r="B22" s="126"/>
-      <c r="C22" s="126"/>
-      <c r="D22" s="127"/>
+      <c r="B22" s="135"/>
+      <c r="C22" s="135"/>
+      <c r="D22" s="136"/>
     </row>
     <row r="23" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B23" s="1" t="s">
@@ -3821,37 +3827,37 @@
       <c r="D24" s="12"/>
     </row>
     <row r="25" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B25" s="112" t="s">
+      <c r="B25" s="133" t="s">
         <v>210</v>
       </c>
-      <c r="C25" s="113"/>
+      <c r="C25" s="134"/>
       <c r="D25" s="12"/>
     </row>
     <row r="26" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B26" s="112" t="s">
+      <c r="B26" s="133" t="s">
         <v>87</v>
       </c>
-      <c r="C26" s="113"/>
+      <c r="C26" s="134"/>
       <c r="D26" s="12"/>
     </row>
     <row r="27" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B27" s="112" t="s">
+      <c r="B27" s="133" t="s">
         <v>64</v>
       </c>
-      <c r="C27" s="113"/>
+      <c r="C27" s="134"/>
       <c r="D27" s="12"/>
     </row>
     <row r="28" spans="2:4" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="136" t="s">
+      <c r="B28" s="141" t="s">
         <v>242</v>
       </c>
-      <c r="C28" s="137"/>
+      <c r="C28" s="142"/>
       <c r="D28" s="12"/>
     </row>
     <row r="29" spans="2:4" ht="18" x14ac:dyDescent="0.35">
-      <c r="B29" s="132"/>
-      <c r="C29" s="132"/>
-      <c r="D29" s="133"/>
+      <c r="B29" s="137"/>
+      <c r="C29" s="137"/>
+      <c r="D29" s="138"/>
     </row>
     <row r="30" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B30" s="1" t="s">
@@ -3868,37 +3874,37 @@
       <c r="D31" s="12"/>
     </row>
     <row r="32" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B32" s="112" t="s">
+      <c r="B32" s="133" t="s">
         <v>212</v>
       </c>
-      <c r="C32" s="113"/>
+      <c r="C32" s="134"/>
       <c r="D32" s="12"/>
     </row>
     <row r="33" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B33" s="112" t="s">
+      <c r="B33" s="133" t="s">
         <v>87</v>
       </c>
-      <c r="C33" s="113"/>
+      <c r="C33" s="134"/>
       <c r="D33" s="12"/>
     </row>
     <row r="34" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B34" s="112" t="s">
+      <c r="B34" s="133" t="s">
         <v>64</v>
       </c>
-      <c r="C34" s="113"/>
+      <c r="C34" s="134"/>
       <c r="D34" s="12"/>
     </row>
     <row r="35" spans="2:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B35" s="134" t="s">
+      <c r="B35" s="139" t="s">
         <v>243</v>
       </c>
-      <c r="C35" s="135"/>
+      <c r="C35" s="140"/>
       <c r="D35" s="12"/>
     </row>
     <row r="36" spans="2:4" ht="18" x14ac:dyDescent="0.35">
-      <c r="B36" s="126"/>
-      <c r="C36" s="126"/>
-      <c r="D36" s="127"/>
+      <c r="B36" s="135"/>
+      <c r="C36" s="135"/>
+      <c r="D36" s="136"/>
     </row>
     <row r="37" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B37" s="1" t="s">
@@ -3908,97 +3914,95 @@
       <c r="D37" s="3"/>
     </row>
     <row r="38" spans="2:4" ht="18" x14ac:dyDescent="0.25">
-      <c r="B38" s="128"/>
-      <c r="C38" s="129"/>
-      <c r="D38" s="130"/>
+      <c r="B38" s="130"/>
+      <c r="C38" s="131"/>
+      <c r="D38" s="132"/>
     </row>
     <row r="39" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B39" s="114" t="s">
+      <c r="B39" s="128" t="s">
         <v>107</v>
       </c>
-      <c r="C39" s="131"/>
+      <c r="C39" s="129"/>
       <c r="D39" s="56"/>
     </row>
     <row r="40" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B40" s="114" t="s">
+      <c r="B40" s="128" t="s">
         <v>108</v>
       </c>
-      <c r="C40" s="131"/>
+      <c r="C40" s="129"/>
       <c r="D40" s="56"/>
     </row>
     <row r="41" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B41" s="114" t="s">
+      <c r="B41" s="128" t="s">
         <v>109</v>
       </c>
-      <c r="C41" s="131"/>
+      <c r="C41" s="129"/>
       <c r="D41" s="56"/>
     </row>
     <row r="42" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B42" s="114" t="s">
+      <c r="B42" s="128" t="s">
         <v>214</v>
       </c>
-      <c r="C42" s="131"/>
+      <c r="C42" s="129"/>
       <c r="D42" s="57"/>
     </row>
     <row r="43" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B43" s="114" t="s">
+      <c r="B43" s="128" t="s">
         <v>110</v>
       </c>
-      <c r="C43" s="131"/>
+      <c r="C43" s="129"/>
       <c r="D43" s="56"/>
     </row>
     <row r="44" spans="2:4" ht="18" x14ac:dyDescent="0.25">
-      <c r="B44" s="128"/>
-      <c r="C44" s="129"/>
-      <c r="D44" s="130"/>
+      <c r="B44" s="130"/>
+      <c r="C44" s="131"/>
+      <c r="D44" s="132"/>
     </row>
     <row r="45" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B45" s="114" t="s">
+      <c r="B45" s="128" t="s">
         <v>107</v>
       </c>
-      <c r="C45" s="131"/>
+      <c r="C45" s="129"/>
       <c r="D45" s="56"/>
     </row>
     <row r="46" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B46" s="114" t="s">
+      <c r="B46" s="128" t="s">
         <v>108</v>
       </c>
-      <c r="C46" s="131"/>
+      <c r="C46" s="129"/>
       <c r="D46" s="56"/>
     </row>
     <row r="47" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B47" s="114" t="s">
+      <c r="B47" s="128" t="s">
         <v>109</v>
       </c>
-      <c r="C47" s="131"/>
+      <c r="C47" s="129"/>
       <c r="D47" s="56"/>
     </row>
     <row r="48" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B48" s="114" t="s">
+      <c r="B48" s="128" t="s">
         <v>214</v>
       </c>
-      <c r="C48" s="131"/>
+      <c r="C48" s="129"/>
       <c r="D48" s="57"/>
     </row>
     <row r="49" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B49" s="114" t="s">
+      <c r="B49" s="128" t="s">
         <v>110</v>
       </c>
-      <c r="C49" s="131"/>
+      <c r="C49" s="129"/>
       <c r="D49" s="56"/>
     </row>
   </sheetData>
   <mergeCells count="32">
-    <mergeCell ref="B46:C46"/>
-    <mergeCell ref="B47:C47"/>
-    <mergeCell ref="B48:C48"/>
-    <mergeCell ref="B49:C49"/>
-    <mergeCell ref="B40:C40"/>
-    <mergeCell ref="B41:C41"/>
-    <mergeCell ref="B42:C42"/>
-    <mergeCell ref="B43:C43"/>
-    <mergeCell ref="B44:D44"/>
-    <mergeCell ref="B45:C45"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B2:D8"/>
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B19:C19"/>
     <mergeCell ref="B21:C21"/>
     <mergeCell ref="B25:C25"/>
     <mergeCell ref="B38:D38"/>
@@ -4013,14 +4017,16 @@
     <mergeCell ref="B26:C26"/>
     <mergeCell ref="B27:C27"/>
     <mergeCell ref="B28:C28"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="B2:D8"/>
-    <mergeCell ref="B9:D9"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="B46:C46"/>
+    <mergeCell ref="B47:C47"/>
+    <mergeCell ref="B48:C48"/>
+    <mergeCell ref="B49:C49"/>
+    <mergeCell ref="B40:C40"/>
+    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="B42:C42"/>
+    <mergeCell ref="B43:C43"/>
+    <mergeCell ref="B44:D44"/>
+    <mergeCell ref="B45:C45"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -4067,11 +4073,11 @@
       <c r="F3" s="8"/>
     </row>
     <row r="4" spans="2:24" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="B4" s="142"/>
-      <c r="C4" s="142"/>
-      <c r="D4" s="142"/>
-      <c r="E4" s="142"/>
-      <c r="F4" s="142"/>
+      <c r="B4" s="170"/>
+      <c r="C4" s="170"/>
+      <c r="D4" s="170"/>
+      <c r="E4" s="170"/>
+      <c r="F4" s="170"/>
     </row>
     <row r="5" spans="2:24" ht="15.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B5" s="20"/>
@@ -4086,16 +4092,16 @@
       <c r="D6" s="21"/>
       <c r="E6" s="21"/>
       <c r="F6" s="21"/>
-      <c r="G6" s="152" t="s">
+      <c r="G6" s="171" t="s">
         <v>200</v>
       </c>
-      <c r="H6" s="153"/>
-      <c r="I6" s="154"/>
-      <c r="V6" s="155" t="s">
+      <c r="H6" s="172"/>
+      <c r="I6" s="173"/>
+      <c r="V6" s="154" t="s">
         <v>240</v>
       </c>
-      <c r="W6" s="156"/>
-      <c r="X6" s="157"/>
+      <c r="W6" s="155"/>
+      <c r="X6" s="156"/>
     </row>
     <row r="7" spans="2:24" ht="16.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B7" s="13"/>
@@ -4110,18 +4116,18 @@
       <c r="D8" s="20"/>
       <c r="E8" s="20"/>
       <c r="F8" s="20"/>
-      <c r="G8" s="143">
+      <c r="G8" s="157">
         <f>AVERAGE(G43:G50)*5</f>
         <v>2.5258318070818078</v>
       </c>
-      <c r="H8" s="144"/>
-      <c r="I8" s="145"/>
-      <c r="V8" s="143" t="e">
+      <c r="H8" s="158"/>
+      <c r="I8" s="159"/>
+      <c r="V8" s="157" t="e">
         <f>AVERAGE(K43:K50)*5</f>
         <v>#REF!</v>
       </c>
-      <c r="W8" s="144"/>
-      <c r="X8" s="145"/>
+      <c r="W8" s="158"/>
+      <c r="X8" s="159"/>
     </row>
     <row r="9" spans="2:24" ht="90.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B9" s="21"/>
@@ -4129,12 +4135,12 @@
       <c r="D9" s="21"/>
       <c r="E9" s="21"/>
       <c r="F9" s="21"/>
-      <c r="G9" s="146"/>
-      <c r="H9" s="147"/>
-      <c r="I9" s="148"/>
-      <c r="V9" s="146"/>
-      <c r="W9" s="147"/>
-      <c r="X9" s="148"/>
+      <c r="G9" s="160"/>
+      <c r="H9" s="161"/>
+      <c r="I9" s="162"/>
+      <c r="V9" s="160"/>
+      <c r="W9" s="161"/>
+      <c r="X9" s="162"/>
     </row>
     <row r="10" spans="2:24" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B10" s="13"/>
@@ -4142,12 +4148,12 @@
       <c r="D10" s="13"/>
       <c r="E10" s="13"/>
       <c r="F10" s="13"/>
-      <c r="G10" s="146"/>
-      <c r="H10" s="147"/>
-      <c r="I10" s="148"/>
-      <c r="V10" s="146"/>
-      <c r="W10" s="147"/>
-      <c r="X10" s="148"/>
+      <c r="G10" s="160"/>
+      <c r="H10" s="161"/>
+      <c r="I10" s="162"/>
+      <c r="V10" s="160"/>
+      <c r="W10" s="161"/>
+      <c r="X10" s="162"/>
     </row>
     <row r="11" spans="2:24" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B11" s="13"/>
@@ -4155,19 +4161,19 @@
       <c r="D11" s="13"/>
       <c r="E11" s="13"/>
       <c r="F11" s="13"/>
-      <c r="G11" s="149"/>
-      <c r="H11" s="150"/>
-      <c r="I11" s="151"/>
-      <c r="V11" s="149"/>
-      <c r="W11" s="150"/>
-      <c r="X11" s="151"/>
+      <c r="G11" s="163"/>
+      <c r="H11" s="164"/>
+      <c r="I11" s="165"/>
+      <c r="V11" s="163"/>
+      <c r="W11" s="164"/>
+      <c r="X11" s="165"/>
     </row>
     <row r="12" spans="2:24" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B12" s="138"/>
-      <c r="C12" s="138"/>
-      <c r="D12" s="138"/>
-      <c r="E12" s="138"/>
-      <c r="F12" s="138"/>
+      <c r="B12" s="166"/>
+      <c r="C12" s="166"/>
+      <c r="D12" s="166"/>
+      <c r="E12" s="166"/>
+      <c r="F12" s="166"/>
     </row>
     <row r="13" spans="2:24" ht="15" x14ac:dyDescent="0.2">
       <c r="B13" s="14"/>
@@ -4191,11 +4197,11 @@
       <c r="F15" s="13"/>
     </row>
     <row r="16" spans="2:24" ht="15.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B16" s="138"/>
-      <c r="C16" s="138"/>
-      <c r="D16" s="138"/>
-      <c r="E16" s="138"/>
-      <c r="F16" s="138"/>
+      <c r="B16" s="166"/>
+      <c r="C16" s="166"/>
+      <c r="D16" s="166"/>
+      <c r="E16" s="166"/>
+      <c r="F16" s="166"/>
     </row>
     <row r="17" spans="2:6" ht="15" x14ac:dyDescent="0.2">
       <c r="B17" s="14"/>
@@ -4248,18 +4254,18 @@
     </row>
     <row r="35" spans="3:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="41" spans="3:11" ht="16.5" x14ac:dyDescent="0.2">
-      <c r="D41" s="139" t="s">
+      <c r="D41" s="167" t="s">
         <v>71</v>
       </c>
-      <c r="E41" s="140"/>
-      <c r="F41" s="140"/>
-      <c r="G41" s="141"/>
-      <c r="H41" s="139" t="s">
+      <c r="E41" s="168"/>
+      <c r="F41" s="168"/>
+      <c r="G41" s="169"/>
+      <c r="H41" s="167" t="s">
         <v>72</v>
       </c>
-      <c r="I41" s="140"/>
-      <c r="J41" s="140"/>
-      <c r="K41" s="141"/>
+      <c r="I41" s="168"/>
+      <c r="J41" s="168"/>
+      <c r="K41" s="169"/>
     </row>
     <row r="42" spans="3:11" x14ac:dyDescent="0.2">
       <c r="D42" s="17" t="s">
@@ -4569,15 +4575,15 @@
     </row>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="B4:F4"/>
+    <mergeCell ref="G8:I11"/>
+    <mergeCell ref="G6:I6"/>
     <mergeCell ref="V6:X6"/>
     <mergeCell ref="V8:X11"/>
     <mergeCell ref="B12:F12"/>
     <mergeCell ref="B16:F16"/>
     <mergeCell ref="D41:G41"/>
     <mergeCell ref="H41:K41"/>
-    <mergeCell ref="B4:F4"/>
-    <mergeCell ref="G8:I11"/>
-    <mergeCell ref="G6:I6"/>
   </mergeCells>
   <conditionalFormatting sqref="F14">
     <cfRule type="iconSet" priority="3">
@@ -4618,8 +4624,8 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="B1:J85"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A63" zoomScale="78" zoomScaleNormal="78" zoomScalePageLayoutView="130" workbookViewId="0">
-      <selection activeCell="G43" sqref="G43"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A44" zoomScale="78" zoomScaleNormal="78" zoomScalePageLayoutView="130" workbookViewId="0">
+      <selection activeCell="J51" sqref="J51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -4631,20 +4637,20 @@
     <col min="5" max="5" width="9.25" customWidth="1"/>
     <col min="6" max="6" width="5.875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="53.5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="30.875" customWidth="1"/>
+    <col min="8" max="8" width="58.125" customWidth="1"/>
     <col min="10" max="11" width="10.875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:8" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B1" s="158" t="s">
+      <c r="B1" s="174" t="s">
         <v>118</v>
       </c>
-      <c r="C1" s="158"/>
-      <c r="D1" s="158"/>
-      <c r="E1" s="158"/>
-      <c r="F1" s="158"/>
-      <c r="G1" s="158"/>
-      <c r="H1" s="158"/>
+      <c r="C1" s="174"/>
+      <c r="D1" s="174"/>
+      <c r="E1" s="174"/>
+      <c r="F1" s="174"/>
+      <c r="G1" s="174"/>
+      <c r="H1" s="174"/>
     </row>
     <row r="2" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B2" s="45"/>
@@ -4712,7 +4718,7 @@
     </row>
     <row r="6" spans="2:8" ht="30" x14ac:dyDescent="0.25">
       <c r="B6" s="31" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C6" s="32" t="s">
         <v>121</v>
@@ -4731,7 +4737,7 @@
     </row>
     <row r="7" spans="2:8" ht="30" x14ac:dyDescent="0.25">
       <c r="B7" s="31" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C7" s="32" t="s">
         <v>122</v>
@@ -4750,7 +4756,7 @@
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B8" s="31" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C8" s="32" t="s">
         <v>120</v>
@@ -4769,7 +4775,7 @@
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B9" s="31" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C9" s="32" t="s">
         <v>123</v>
@@ -4788,7 +4794,7 @@
     </row>
     <row r="10" spans="2:8" ht="30" x14ac:dyDescent="0.25">
       <c r="B10" s="31" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C10" s="32" t="s">
         <v>124</v>
@@ -4826,7 +4832,7 @@
     </row>
     <row r="12" spans="2:8" ht="30" x14ac:dyDescent="0.25">
       <c r="B12" s="31" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C12" s="32" t="s">
         <v>126</v>
@@ -4845,7 +4851,7 @@
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B13" s="31" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C13" s="32" t="s">
         <v>127</v>
@@ -5124,8 +5130,9 @@
       <c r="F27" s="33" t="s">
         <v>63</v>
       </c>
-      <c r="G27" s="170" t="s">
-        <v>255</v>
+      <c r="G27" s="176" t="str">
+        <f>HYPERLINK(CONCATENATE(BASE_URL,"0x04i-Testing-user-interaction.md#testing-user-education"),"Eduction d'utilisateur")</f>
+        <v>Eduction d'utilisateur</v>
       </c>
       <c r="H27" s="66"/>
     </row>
@@ -5564,7 +5571,10 @@
         <f>HYPERLINK(CONCATENATE(BASE_URL,"0x05g-Testing-Network-Communication.md#testing-endpoint-identify-verification"),"Tester la vérification du validité du point terminal")</f>
         <v>Tester la vérification du validité du point terminal</v>
       </c>
-      <c r="H50" s="66"/>
+      <c r="H50" s="178" t="str">
+        <f>HYPERLINK(CONCATENATE(BASE_URL,"0x04f-Testing-Network-Communication.md#making-sure-that-critical-operations-use-secure-communication-channels"),"Assurer que les opérations critiques utilisent des canals de communications sécurisés")</f>
+        <v>Assurer que les opérations critiques utilisent des canals de communications sécurisés</v>
+      </c>
     </row>
     <row r="51" spans="2:8" ht="45" x14ac:dyDescent="0.25">
       <c r="B51" s="50" t="s">
@@ -5608,7 +5618,7 @@
     </row>
     <row r="53" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B53" s="50" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C53" s="51" t="s">
         <v>163</v>
@@ -5761,7 +5771,7 @@
     </row>
     <row r="61" spans="2:8" ht="30" x14ac:dyDescent="0.25">
       <c r="B61" s="50" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="C61" s="51" t="s">
         <v>170</v>
@@ -5781,7 +5791,7 @@
     </row>
     <row r="62" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B62" s="50" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C62" s="51" t="s">
         <v>171</v>
@@ -6130,7 +6140,7 @@
   <mergeCells count="1">
     <mergeCell ref="B1:H1"/>
   </mergeCells>
-  <dataValidations count="2">
+  <dataValidations disablePrompts="1" count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F74:F1048576 H74:H1048576" xr:uid="{00000000-0002-0000-0200-000000000000}">
       <formula1>"Yes,No,N/A"</formula1>
     </dataValidation>
@@ -6151,8 +6161,8 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="B1:G29"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="91" zoomScaleNormal="91" zoomScalePageLayoutView="130" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView showGridLines="0" topLeftCell="A8" zoomScale="91" zoomScaleNormal="91" zoomScalePageLayoutView="130" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -6216,7 +6226,7 @@
     </row>
     <row r="5" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B5" s="72" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C5" s="73" t="s">
         <v>185</v>
@@ -6235,7 +6245,7 @@
     </row>
     <row r="6" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B6" s="72" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="C6" s="73" t="s">
         <v>186</v>
@@ -6254,7 +6264,7 @@
     </row>
     <row r="7" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B7" s="72" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C7" s="73" t="s">
         <v>187</v>
@@ -6273,7 +6283,7 @@
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B8" s="72" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="C8" s="73" t="s">
         <v>188</v>
@@ -6292,7 +6302,7 @@
     </row>
     <row r="9" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B9" s="72" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C9" s="73" t="s">
         <v>189</v>
@@ -6311,7 +6321,7 @@
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B10" s="72" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="C10" s="73" t="s">
         <v>190</v>
@@ -6330,7 +6340,7 @@
     </row>
     <row r="11" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B11" s="72" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="C11" s="73" t="s">
         <v>191</v>
@@ -6341,14 +6351,14 @@
       <c r="E11" s="75" t="s">
         <v>63</v>
       </c>
-      <c r="F11" s="172" t="s">
-        <v>278</v>
+      <c r="F11" s="124" t="s">
+        <v>277</v>
       </c>
       <c r="G11" s="73"/>
     </row>
     <row r="12" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B12" s="72" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="C12" s="73" t="s">
         <v>192</v>
@@ -6359,14 +6369,14 @@
       <c r="E12" s="75" t="s">
         <v>63</v>
       </c>
-      <c r="F12" s="171" t="s">
+      <c r="F12" s="123" t="s">
         <v>75</v>
       </c>
       <c r="G12" s="73"/>
     </row>
     <row r="13" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B13" s="72" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C13" s="73" t="s">
         <v>193</v>
@@ -6424,7 +6434,7 @@
     </row>
     <row r="17" spans="2:7" ht="45" x14ac:dyDescent="0.25">
       <c r="B17" s="72" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="C17" s="73" t="s">
         <v>195</v>
@@ -6435,14 +6445,15 @@
       <c r="E17" s="75" t="s">
         <v>63</v>
       </c>
-      <c r="F17" s="171" t="s">
-        <v>75</v>
+      <c r="F17" s="177" t="str">
+        <f>HYPERLINK(CONCATENATE(BASE_URL,"0x05j-Testing-Resiliency-Against-Reverse-Engineering.md#testing-obfuscation"),"Tester l'Obfuscation")</f>
+        <v>Tester l'Obfuscation</v>
       </c>
       <c r="G17" s="73"/>
     </row>
     <row r="18" spans="2:7" ht="75" x14ac:dyDescent="0.25">
       <c r="B18" s="72" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C18" s="73" t="s">
         <v>196</v>
@@ -6453,8 +6464,8 @@
       <c r="E18" s="75" t="s">
         <v>63</v>
       </c>
-      <c r="F18" s="171" t="s">
-        <v>278</v>
+      <c r="F18" s="123" t="s">
+        <v>277</v>
       </c>
       <c r="G18" s="73"/>
     </row>
@@ -6597,15 +6608,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:8" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B1" s="158" t="s">
+      <c r="B1" s="174" t="s">
         <v>197</v>
       </c>
-      <c r="C1" s="158"/>
-      <c r="D1" s="158"/>
-      <c r="E1" s="158"/>
-      <c r="F1" s="158"/>
-      <c r="G1" s="158"/>
-      <c r="H1" s="158"/>
+      <c r="C1" s="174"/>
+      <c r="D1" s="174"/>
+      <c r="E1" s="174"/>
+      <c r="F1" s="174"/>
+      <c r="G1" s="174"/>
+      <c r="H1" s="174"/>
     </row>
     <row r="2" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B2" s="45"/>
@@ -6673,7 +6684,7 @@
     </row>
     <row r="6" spans="2:8" ht="30" x14ac:dyDescent="0.25">
       <c r="B6" s="31" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C6" s="32" t="s">
         <v>121</v>
@@ -6692,7 +6703,7 @@
     </row>
     <row r="7" spans="2:8" ht="30" x14ac:dyDescent="0.25">
       <c r="B7" s="31" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C7" s="32" t="s">
         <v>122</v>
@@ -6711,7 +6722,7 @@
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B8" s="31" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C8" s="32" t="s">
         <v>120</v>
@@ -6730,7 +6741,7 @@
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B9" s="31" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C9" s="32" t="s">
         <v>123</v>
@@ -6749,7 +6760,7 @@
     </row>
     <row r="10" spans="2:8" ht="30" x14ac:dyDescent="0.25">
       <c r="B10" s="31" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C10" s="32" t="s">
         <v>124</v>
@@ -6787,7 +6798,7 @@
     </row>
     <row r="12" spans="2:8" ht="30" x14ac:dyDescent="0.25">
       <c r="B12" s="31" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C12" s="32" t="s">
         <v>126</v>
@@ -6806,7 +6817,7 @@
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B13" s="31" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C13" s="32" t="s">
         <v>127</v>
@@ -7085,8 +7096,8 @@
       <c r="F27" s="33" t="s">
         <v>63</v>
       </c>
-      <c r="G27" s="170" t="s">
-        <v>256</v>
+      <c r="G27" s="122" t="s">
+        <v>255</v>
       </c>
       <c r="H27" s="66"/>
     </row>
@@ -7448,7 +7459,7 @@
       <c r="F46" s="33" t="s">
         <v>63</v>
       </c>
-      <c r="G46" s="173" t="s">
+      <c r="G46" s="125" t="s">
         <v>75</v>
       </c>
       <c r="H46" s="66"/>
@@ -7568,7 +7579,7 @@
     </row>
     <row r="53" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B53" s="50" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C53" s="51" t="s">
         <v>163</v>
@@ -7580,7 +7591,7 @@
       <c r="F53" s="33" t="s">
         <v>63</v>
       </c>
-      <c r="G53" s="169" t="s">
+      <c r="G53" s="121" t="s">
         <v>254</v>
       </c>
       <c r="H53" s="66"/>
@@ -7672,7 +7683,7 @@
         <v>3</v>
       </c>
       <c r="F58" s="33"/>
-      <c r="G58" s="168" t="s">
+      <c r="G58" s="120" t="s">
         <v>75</v>
       </c>
       <c r="H58" s="66"/>
@@ -7719,7 +7730,7 @@
     </row>
     <row r="61" spans="2:8" ht="30" x14ac:dyDescent="0.25">
       <c r="B61" s="50" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="C61" s="51" t="s">
         <v>170</v>
@@ -7739,7 +7750,7 @@
     </row>
     <row r="62" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B62" s="50" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C62" s="51" t="s">
         <v>171</v>
@@ -8106,7 +8117,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="B1:G29"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" zoomScale="71" zoomScaleNormal="71" zoomScalePageLayoutView="130" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A7" zoomScale="71" zoomScaleNormal="71" zoomScalePageLayoutView="130" workbookViewId="0">
       <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
@@ -8171,7 +8182,7 @@
     </row>
     <row r="5" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B5" s="72" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C5" s="73" t="s">
         <v>185</v>
@@ -8190,7 +8201,7 @@
     </row>
     <row r="6" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B6" s="72" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="C6" s="73" t="s">
         <v>186</v>
@@ -8209,7 +8220,7 @@
     </row>
     <row r="7" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B7" s="72" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C7" s="73" t="s">
         <v>187</v>
@@ -8228,7 +8239,7 @@
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B8" s="72" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="C8" s="73" t="s">
         <v>188</v>
@@ -8239,14 +8250,14 @@
       <c r="E8" s="75" t="s">
         <v>63</v>
       </c>
-      <c r="F8" s="175" t="s">
+      <c r="F8" s="127" t="s">
         <v>75</v>
       </c>
       <c r="G8" s="73"/>
     </row>
     <row r="9" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B9" s="72" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C9" s="73" t="s">
         <v>189</v>
@@ -8257,14 +8268,14 @@
       <c r="E9" s="75" t="s">
         <v>63</v>
       </c>
-      <c r="F9" s="174" t="s">
+      <c r="F9" s="126" t="s">
         <v>75</v>
       </c>
       <c r="G9" s="73"/>
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B10" s="72" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="C10" s="73" t="s">
         <v>190</v>
@@ -8275,14 +8286,14 @@
       <c r="E10" s="75" t="s">
         <v>63</v>
       </c>
-      <c r="F10" s="175" t="s">
+      <c r="F10" s="127" t="s">
         <v>75</v>
       </c>
       <c r="G10" s="73"/>
     </row>
     <row r="11" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B11" s="72" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="C11" s="73" t="s">
         <v>191</v>
@@ -8293,14 +8304,14 @@
       <c r="E11" s="75" t="s">
         <v>63</v>
       </c>
-      <c r="F11" s="171" t="s">
+      <c r="F11" s="123" t="s">
         <v>75</v>
       </c>
       <c r="G11" s="73"/>
     </row>
     <row r="12" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B12" s="72" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="C12" s="73" t="s">
         <v>192</v>
@@ -8311,14 +8322,14 @@
       <c r="E12" s="75" t="s">
         <v>63</v>
       </c>
-      <c r="F12" s="171" t="s">
+      <c r="F12" s="123" t="s">
         <v>75</v>
       </c>
       <c r="G12" s="73"/>
     </row>
     <row r="13" spans="2:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B13" s="72" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C13" s="73" t="s">
         <v>193</v>
@@ -8329,7 +8340,7 @@
       <c r="E13" s="75" t="s">
         <v>63</v>
       </c>
-      <c r="F13" s="174" t="s">
+      <c r="F13" s="126" t="s">
         <v>75</v>
       </c>
       <c r="G13" s="73"/>
@@ -8375,7 +8386,7 @@
     </row>
     <row r="17" spans="2:7" ht="45" x14ac:dyDescent="0.25">
       <c r="B17" s="72" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="C17" s="73" t="s">
         <v>195</v>
@@ -8386,14 +8397,14 @@
       <c r="E17" s="75" t="s">
         <v>63</v>
       </c>
-      <c r="F17" s="171" t="s">
+      <c r="F17" s="123" t="s">
         <v>75</v>
       </c>
       <c r="G17" s="73"/>
     </row>
     <row r="18" spans="2:7" ht="75" x14ac:dyDescent="0.25">
       <c r="B18" s="72" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C18" s="73" t="s">
         <v>196</v>
@@ -8404,7 +8415,7 @@
       <c r="E18" s="75" t="s">
         <v>63</v>
       </c>
-      <c r="F18" s="171" t="s">
+      <c r="F18" s="123" t="s">
         <v>75</v>
       </c>
       <c r="G18" s="73"/>
@@ -8543,10 +8554,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="159" t="s">
+      <c r="A1" s="175" t="s">
         <v>106</v>
       </c>
-      <c r="B1" s="159"/>
+      <c r="B1" s="175"/>
       <c r="C1" s="107"/>
       <c r="D1" s="45"/>
       <c r="E1" s="45"/>
@@ -8761,7 +8772,7 @@
       <c r="D15" s="106">
         <v>43471</v>
       </c>
-      <c r="E15" s="167" t="s">
+      <c r="E15" s="119" t="s">
         <v>252</v>
       </c>
     </row>
@@ -8783,36 +8794,36 @@
       </c>
     </row>
     <row r="17" spans="1:5" ht="135.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="161" t="s">
+      <c r="A17" s="113" t="s">
         <v>248</v>
       </c>
-      <c r="B17" s="162" t="s">
+      <c r="B17" s="114" t="s">
         <v>249</v>
       </c>
-      <c r="C17" s="162" t="s">
+      <c r="C17" s="114" t="s">
         <v>232</v>
       </c>
-      <c r="D17" s="163">
+      <c r="D17" s="115">
         <v>43476</v>
       </c>
-      <c r="E17" s="166" t="s">
+      <c r="E17" s="118" t="s">
         <v>251</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="160" t="s">
+      <c r="A18" s="112" t="s">
         <v>104</v>
       </c>
-      <c r="B18" s="164" t="s">
+      <c r="B18" s="116" t="s">
         <v>250</v>
       </c>
-      <c r="C18" s="164" t="s">
+      <c r="C18" s="116" t="s">
         <v>232</v>
       </c>
-      <c r="D18" s="165">
+      <c r="D18" s="117">
         <v>43478</v>
       </c>
-      <c r="E18" s="160" t="s">
+      <c r="E18" s="112" t="s">
         <v>253</v>
       </c>
     </row>

</xml_diff>